<commit_message>
* Fix problem of Insert new rows into tabular data of excel. * Upgrade to 1.2.3
Signed-off-by: gengxuehong <gengxuehong@foxmail.com>
</commit_message>
<xml_diff>
--- a/Develop/Giga/Giga.Test/Transformer/TransformerTest.xlsx
+++ b/Develop/Giga/Giga.Test/Transformer/TransformerTest.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -12,9 +12,12 @@
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
+    <definedName name="DATA_RANGE">Sheet1!$A$4:$J$12</definedName>
     <definedName name="DELIVERY">'SG Purchase Order'!$AC$19</definedName>
     <definedName name="END_OF_DATA">Sheet1!$B$10</definedName>
+    <definedName name="END_OF_FILE">Sheet1!$A$12</definedName>
     <definedName name="END_OF_ITEMS">'SG Purchase Order'!$B$34</definedName>
+    <definedName name="ENDOFDATA">Sheet1!$A$12</definedName>
     <definedName name="EXT_PO">'SG Purchase Order'!$AC$16</definedName>
     <definedName name="INCOTERMS">'SG Purchase Order'!$AC$20</definedName>
     <definedName name="PAYMENT">'SG Purchase Order'!$AC$18</definedName>
@@ -672,6 +675,9 @@
     <xf numFmtId="4" fontId="3" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -737,9 +743,6 @@
     </xf>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1093,8 +1096,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -1416,6 +1419,22 @@
       <c r="A12" t="s">
         <v>28</v>
       </c>
+      <c r="E12" s="4">
+        <f>SUM(E4:E11)</f>
+        <v>187.64799999999997</v>
+      </c>
+      <c r="F12">
+        <f>AVERAGE(F4:F11)</f>
+        <v>45</v>
+      </c>
+      <c r="G12" s="4">
+        <f>SUM(G4:G11)</f>
+        <v>865.84</v>
+      </c>
+      <c r="H12">
+        <f>AVERAGE(H4:H11)</f>
+        <v>4870.3500000000004</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
@@ -1428,7 +1447,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AO45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A32" workbookViewId="0">
+    <sheetView topLeftCell="A32" workbookViewId="0">
       <selection activeCell="L33" sqref="L33:P33"/>
     </sheetView>
   </sheetViews>
@@ -1454,37 +1473,37 @@
       <c r="D1" s="6"/>
       <c r="E1" s="6"/>
       <c r="F1" s="6"/>
-      <c r="G1" s="70"/>
-      <c r="H1" s="70"/>
-      <c r="I1" s="70"/>
-      <c r="J1" s="70"/>
-      <c r="K1" s="70"/>
-      <c r="L1" s="70"/>
-      <c r="M1" s="70"/>
-      <c r="N1" s="70"/>
-      <c r="O1" s="70"/>
-      <c r="P1" s="70"/>
-      <c r="Q1" s="70"/>
-      <c r="R1" s="70"/>
-      <c r="S1" s="70"/>
-      <c r="T1" s="70"/>
-      <c r="U1" s="70"/>
-      <c r="V1" s="70"/>
-      <c r="W1" s="70"/>
-      <c r="X1" s="70"/>
-      <c r="Y1" s="70"/>
-      <c r="Z1" s="70"/>
-      <c r="AA1" s="70"/>
-      <c r="AB1" s="70"/>
-      <c r="AC1" s="70"/>
-      <c r="AD1" s="70"/>
-      <c r="AE1" s="70"/>
-      <c r="AF1" s="70"/>
-      <c r="AG1" s="70"/>
-      <c r="AH1" s="70"/>
-      <c r="AI1" s="70"/>
-      <c r="AJ1" s="70"/>
-      <c r="AK1" s="70"/>
+      <c r="G1" s="71"/>
+      <c r="H1" s="71"/>
+      <c r="I1" s="71"/>
+      <c r="J1" s="71"/>
+      <c r="K1" s="71"/>
+      <c r="L1" s="71"/>
+      <c r="M1" s="71"/>
+      <c r="N1" s="71"/>
+      <c r="O1" s="71"/>
+      <c r="P1" s="71"/>
+      <c r="Q1" s="71"/>
+      <c r="R1" s="71"/>
+      <c r="S1" s="71"/>
+      <c r="T1" s="71"/>
+      <c r="U1" s="71"/>
+      <c r="V1" s="71"/>
+      <c r="W1" s="71"/>
+      <c r="X1" s="71"/>
+      <c r="Y1" s="71"/>
+      <c r="Z1" s="71"/>
+      <c r="AA1" s="71"/>
+      <c r="AB1" s="71"/>
+      <c r="AC1" s="71"/>
+      <c r="AD1" s="71"/>
+      <c r="AE1" s="71"/>
+      <c r="AF1" s="71"/>
+      <c r="AG1" s="71"/>
+      <c r="AH1" s="71"/>
+      <c r="AI1" s="71"/>
+      <c r="AJ1" s="71"/>
+      <c r="AK1" s="71"/>
       <c r="AL1" s="6"/>
       <c r="AM1" s="6"/>
       <c r="AN1" s="6"/>
@@ -1497,40 +1516,40 @@
       <c r="D2" s="6"/>
       <c r="E2" s="6"/>
       <c r="F2" s="6"/>
-      <c r="G2" s="71" t="s">
+      <c r="G2" s="72" t="s">
         <v>29</v>
       </c>
-      <c r="H2" s="72"/>
-      <c r="I2" s="72"/>
-      <c r="J2" s="72"/>
-      <c r="K2" s="72"/>
-      <c r="L2" s="72"/>
-      <c r="M2" s="72"/>
-      <c r="N2" s="72"/>
-      <c r="O2" s="72"/>
-      <c r="P2" s="72"/>
-      <c r="Q2" s="72"/>
-      <c r="R2" s="72"/>
-      <c r="S2" s="72"/>
-      <c r="T2" s="72"/>
-      <c r="U2" s="72"/>
-      <c r="V2" s="72"/>
-      <c r="W2" s="72"/>
-      <c r="X2" s="72"/>
-      <c r="Y2" s="72"/>
-      <c r="Z2" s="72"/>
-      <c r="AA2" s="72"/>
-      <c r="AB2" s="72"/>
-      <c r="AC2" s="72"/>
-      <c r="AD2" s="72"/>
-      <c r="AE2" s="72"/>
-      <c r="AF2" s="72"/>
-      <c r="AG2" s="72"/>
-      <c r="AH2" s="72"/>
-      <c r="AI2" s="72"/>
-      <c r="AJ2" s="72"/>
-      <c r="AK2" s="72"/>
-      <c r="AL2" s="72"/>
+      <c r="H2" s="73"/>
+      <c r="I2" s="73"/>
+      <c r="J2" s="73"/>
+      <c r="K2" s="73"/>
+      <c r="L2" s="73"/>
+      <c r="M2" s="73"/>
+      <c r="N2" s="73"/>
+      <c r="O2" s="73"/>
+      <c r="P2" s="73"/>
+      <c r="Q2" s="73"/>
+      <c r="R2" s="73"/>
+      <c r="S2" s="73"/>
+      <c r="T2" s="73"/>
+      <c r="U2" s="73"/>
+      <c r="V2" s="73"/>
+      <c r="W2" s="73"/>
+      <c r="X2" s="73"/>
+      <c r="Y2" s="73"/>
+      <c r="Z2" s="73"/>
+      <c r="AA2" s="73"/>
+      <c r="AB2" s="73"/>
+      <c r="AC2" s="73"/>
+      <c r="AD2" s="73"/>
+      <c r="AE2" s="73"/>
+      <c r="AF2" s="73"/>
+      <c r="AG2" s="73"/>
+      <c r="AH2" s="73"/>
+      <c r="AI2" s="73"/>
+      <c r="AJ2" s="73"/>
+      <c r="AK2" s="73"/>
+      <c r="AL2" s="73"/>
       <c r="AM2" s="6"/>
       <c r="AN2" s="6"/>
       <c r="AO2" s="6"/>
@@ -1542,40 +1561,40 @@
       <c r="D3" s="6"/>
       <c r="E3" s="6"/>
       <c r="F3" s="6"/>
-      <c r="G3" s="70" t="s">
+      <c r="G3" s="71" t="s">
         <v>30</v>
       </c>
-      <c r="H3" s="70"/>
-      <c r="I3" s="70"/>
-      <c r="J3" s="70"/>
-      <c r="K3" s="70"/>
-      <c r="L3" s="70"/>
-      <c r="M3" s="70"/>
-      <c r="N3" s="70"/>
-      <c r="O3" s="70"/>
-      <c r="P3" s="70"/>
-      <c r="Q3" s="70"/>
-      <c r="R3" s="70"/>
-      <c r="S3" s="70"/>
-      <c r="T3" s="70"/>
-      <c r="U3" s="70"/>
-      <c r="V3" s="70"/>
-      <c r="W3" s="70"/>
-      <c r="X3" s="70"/>
-      <c r="Y3" s="70"/>
-      <c r="Z3" s="70"/>
-      <c r="AA3" s="70"/>
-      <c r="AB3" s="70"/>
-      <c r="AC3" s="70"/>
-      <c r="AD3" s="70"/>
-      <c r="AE3" s="70"/>
-      <c r="AF3" s="70"/>
-      <c r="AG3" s="70"/>
-      <c r="AH3" s="70"/>
-      <c r="AI3" s="70"/>
-      <c r="AJ3" s="70"/>
-      <c r="AK3" s="70"/>
-      <c r="AL3" s="70"/>
+      <c r="H3" s="71"/>
+      <c r="I3" s="71"/>
+      <c r="J3" s="71"/>
+      <c r="K3" s="71"/>
+      <c r="L3" s="71"/>
+      <c r="M3" s="71"/>
+      <c r="N3" s="71"/>
+      <c r="O3" s="71"/>
+      <c r="P3" s="71"/>
+      <c r="Q3" s="71"/>
+      <c r="R3" s="71"/>
+      <c r="S3" s="71"/>
+      <c r="T3" s="71"/>
+      <c r="U3" s="71"/>
+      <c r="V3" s="71"/>
+      <c r="W3" s="71"/>
+      <c r="X3" s="71"/>
+      <c r="Y3" s="71"/>
+      <c r="Z3" s="71"/>
+      <c r="AA3" s="71"/>
+      <c r="AB3" s="71"/>
+      <c r="AC3" s="71"/>
+      <c r="AD3" s="71"/>
+      <c r="AE3" s="71"/>
+      <c r="AF3" s="71"/>
+      <c r="AG3" s="71"/>
+      <c r="AH3" s="71"/>
+      <c r="AI3" s="71"/>
+      <c r="AJ3" s="71"/>
+      <c r="AK3" s="71"/>
+      <c r="AL3" s="71"/>
       <c r="AM3" s="6"/>
       <c r="AN3" s="6"/>
       <c r="AO3" s="6"/>
@@ -1587,40 +1606,40 @@
       <c r="D4" s="6"/>
       <c r="E4" s="6"/>
       <c r="F4" s="6"/>
-      <c r="G4" s="73" t="s">
+      <c r="G4" s="74" t="s">
         <v>31</v>
       </c>
-      <c r="H4" s="73"/>
-      <c r="I4" s="73"/>
-      <c r="J4" s="73"/>
-      <c r="K4" s="73"/>
-      <c r="L4" s="73"/>
-      <c r="M4" s="73"/>
-      <c r="N4" s="73"/>
-      <c r="O4" s="73"/>
-      <c r="P4" s="73"/>
-      <c r="Q4" s="73"/>
-      <c r="R4" s="73"/>
-      <c r="S4" s="73"/>
-      <c r="T4" s="73"/>
-      <c r="U4" s="73"/>
-      <c r="V4" s="73"/>
-      <c r="W4" s="73"/>
-      <c r="X4" s="73"/>
-      <c r="Y4" s="73"/>
-      <c r="Z4" s="73"/>
-      <c r="AA4" s="73"/>
-      <c r="AB4" s="73"/>
-      <c r="AC4" s="73"/>
-      <c r="AD4" s="73"/>
-      <c r="AE4" s="73"/>
-      <c r="AF4" s="73"/>
-      <c r="AG4" s="73"/>
-      <c r="AH4" s="73"/>
-      <c r="AI4" s="73"/>
-      <c r="AJ4" s="73"/>
-      <c r="AK4" s="73"/>
-      <c r="AL4" s="73"/>
+      <c r="H4" s="74"/>
+      <c r="I4" s="74"/>
+      <c r="J4" s="74"/>
+      <c r="K4" s="74"/>
+      <c r="L4" s="74"/>
+      <c r="M4" s="74"/>
+      <c r="N4" s="74"/>
+      <c r="O4" s="74"/>
+      <c r="P4" s="74"/>
+      <c r="Q4" s="74"/>
+      <c r="R4" s="74"/>
+      <c r="S4" s="74"/>
+      <c r="T4" s="74"/>
+      <c r="U4" s="74"/>
+      <c r="V4" s="74"/>
+      <c r="W4" s="74"/>
+      <c r="X4" s="74"/>
+      <c r="Y4" s="74"/>
+      <c r="Z4" s="74"/>
+      <c r="AA4" s="74"/>
+      <c r="AB4" s="74"/>
+      <c r="AC4" s="74"/>
+      <c r="AD4" s="74"/>
+      <c r="AE4" s="74"/>
+      <c r="AF4" s="74"/>
+      <c r="AG4" s="74"/>
+      <c r="AH4" s="74"/>
+      <c r="AI4" s="74"/>
+      <c r="AJ4" s="74"/>
+      <c r="AK4" s="74"/>
+      <c r="AL4" s="74"/>
       <c r="AM4" s="6"/>
       <c r="AN4" s="6"/>
       <c r="AO4" s="6"/>
@@ -1660,17 +1679,17 @@
       <c r="AD5" s="10"/>
       <c r="AE5" s="10"/>
       <c r="AF5" s="10"/>
-      <c r="AG5" s="74" t="s">
+      <c r="AG5" s="75" t="s">
         <v>33</v>
       </c>
-      <c r="AH5" s="74"/>
-      <c r="AI5" s="74"/>
-      <c r="AJ5" s="74"/>
-      <c r="AK5" s="74"/>
-      <c r="AL5" s="74"/>
-      <c r="AM5" s="74"/>
-      <c r="AN5" s="74"/>
-      <c r="AO5" s="75"/>
+      <c r="AH5" s="75"/>
+      <c r="AI5" s="75"/>
+      <c r="AJ5" s="75"/>
+      <c r="AK5" s="75"/>
+      <c r="AL5" s="75"/>
+      <c r="AM5" s="75"/>
+      <c r="AN5" s="75"/>
+      <c r="AO5" s="76"/>
     </row>
     <row r="6" spans="1:41" ht="12.75">
       <c r="A6" s="6"/>
@@ -1740,11 +1759,11 @@
       <c r="T7" s="17"/>
       <c r="U7" s="17"/>
       <c r="V7" s="15"/>
-      <c r="W7" s="69" t="s">
+      <c r="W7" s="70" t="s">
         <v>35</v>
       </c>
-      <c r="X7" s="69"/>
-      <c r="Y7" s="69"/>
+      <c r="X7" s="70"/>
+      <c r="Y7" s="70"/>
       <c r="Z7" s="17"/>
       <c r="AA7" s="17"/>
       <c r="AB7" s="17"/>
@@ -1765,263 +1784,263 @@
     <row r="8" spans="1:41" ht="12.75">
       <c r="A8" s="6"/>
       <c r="B8" s="15"/>
-      <c r="C8" s="64" t="s">
+      <c r="C8" s="65" t="s">
         <v>36</v>
       </c>
-      <c r="D8" s="65"/>
-      <c r="E8" s="65"/>
-      <c r="F8" s="65"/>
-      <c r="G8" s="65"/>
-      <c r="H8" s="65"/>
-      <c r="I8" s="65"/>
-      <c r="J8" s="65"/>
-      <c r="K8" s="65"/>
-      <c r="L8" s="65"/>
-      <c r="M8" s="65"/>
-      <c r="N8" s="65"/>
-      <c r="O8" s="65"/>
-      <c r="P8" s="65"/>
-      <c r="Q8" s="65"/>
-      <c r="R8" s="65"/>
-      <c r="S8" s="65"/>
-      <c r="T8" s="65"/>
+      <c r="D8" s="66"/>
+      <c r="E8" s="66"/>
+      <c r="F8" s="66"/>
+      <c r="G8" s="66"/>
+      <c r="H8" s="66"/>
+      <c r="I8" s="66"/>
+      <c r="J8" s="66"/>
+      <c r="K8" s="66"/>
+      <c r="L8" s="66"/>
+      <c r="M8" s="66"/>
+      <c r="N8" s="66"/>
+      <c r="O8" s="66"/>
+      <c r="P8" s="66"/>
+      <c r="Q8" s="66"/>
+      <c r="R8" s="66"/>
+      <c r="S8" s="66"/>
+      <c r="T8" s="66"/>
       <c r="U8" s="17"/>
       <c r="V8" s="15"/>
-      <c r="W8" s="64" t="s">
+      <c r="W8" s="65" t="s">
         <v>37</v>
       </c>
-      <c r="X8" s="65"/>
-      <c r="Y8" s="65"/>
-      <c r="Z8" s="65"/>
-      <c r="AA8" s="65"/>
-      <c r="AB8" s="65"/>
-      <c r="AC8" s="65"/>
-      <c r="AD8" s="65"/>
-      <c r="AE8" s="65"/>
-      <c r="AF8" s="65"/>
-      <c r="AG8" s="65"/>
-      <c r="AH8" s="65"/>
-      <c r="AI8" s="65"/>
-      <c r="AJ8" s="65"/>
-      <c r="AK8" s="65"/>
-      <c r="AL8" s="65"/>
-      <c r="AM8" s="65"/>
-      <c r="AN8" s="65"/>
+      <c r="X8" s="66"/>
+      <c r="Y8" s="66"/>
+      <c r="Z8" s="66"/>
+      <c r="AA8" s="66"/>
+      <c r="AB8" s="66"/>
+      <c r="AC8" s="66"/>
+      <c r="AD8" s="66"/>
+      <c r="AE8" s="66"/>
+      <c r="AF8" s="66"/>
+      <c r="AG8" s="66"/>
+      <c r="AH8" s="66"/>
+      <c r="AI8" s="66"/>
+      <c r="AJ8" s="66"/>
+      <c r="AK8" s="66"/>
+      <c r="AL8" s="66"/>
+      <c r="AM8" s="66"/>
+      <c r="AN8" s="66"/>
       <c r="AO8" s="18"/>
     </row>
     <row r="9" spans="1:41" ht="12.75">
       <c r="A9" s="6"/>
       <c r="B9" s="15"/>
-      <c r="C9" s="65"/>
-      <c r="D9" s="65"/>
-      <c r="E9" s="65"/>
-      <c r="F9" s="65"/>
-      <c r="G9" s="65"/>
-      <c r="H9" s="65"/>
-      <c r="I9" s="65"/>
-      <c r="J9" s="65"/>
-      <c r="K9" s="65"/>
-      <c r="L9" s="65"/>
-      <c r="M9" s="65"/>
-      <c r="N9" s="65"/>
-      <c r="O9" s="65"/>
-      <c r="P9" s="65"/>
-      <c r="Q9" s="65"/>
-      <c r="R9" s="65"/>
-      <c r="S9" s="65"/>
-      <c r="T9" s="65"/>
+      <c r="C9" s="66"/>
+      <c r="D9" s="66"/>
+      <c r="E9" s="66"/>
+      <c r="F9" s="66"/>
+      <c r="G9" s="66"/>
+      <c r="H9" s="66"/>
+      <c r="I9" s="66"/>
+      <c r="J9" s="66"/>
+      <c r="K9" s="66"/>
+      <c r="L9" s="66"/>
+      <c r="M9" s="66"/>
+      <c r="N9" s="66"/>
+      <c r="O9" s="66"/>
+      <c r="P9" s="66"/>
+      <c r="Q9" s="66"/>
+      <c r="R9" s="66"/>
+      <c r="S9" s="66"/>
+      <c r="T9" s="66"/>
       <c r="U9" s="17"/>
       <c r="V9" s="15"/>
-      <c r="W9" s="65"/>
-      <c r="X9" s="65"/>
-      <c r="Y9" s="65"/>
-      <c r="Z9" s="65"/>
-      <c r="AA9" s="65"/>
-      <c r="AB9" s="65"/>
-      <c r="AC9" s="65"/>
-      <c r="AD9" s="65"/>
-      <c r="AE9" s="65"/>
-      <c r="AF9" s="65"/>
-      <c r="AG9" s="65"/>
-      <c r="AH9" s="65"/>
-      <c r="AI9" s="65"/>
-      <c r="AJ9" s="65"/>
-      <c r="AK9" s="65"/>
-      <c r="AL9" s="65"/>
-      <c r="AM9" s="65"/>
-      <c r="AN9" s="65"/>
+      <c r="W9" s="66"/>
+      <c r="X9" s="66"/>
+      <c r="Y9" s="66"/>
+      <c r="Z9" s="66"/>
+      <c r="AA9" s="66"/>
+      <c r="AB9" s="66"/>
+      <c r="AC9" s="66"/>
+      <c r="AD9" s="66"/>
+      <c r="AE9" s="66"/>
+      <c r="AF9" s="66"/>
+      <c r="AG9" s="66"/>
+      <c r="AH9" s="66"/>
+      <c r="AI9" s="66"/>
+      <c r="AJ9" s="66"/>
+      <c r="AK9" s="66"/>
+      <c r="AL9" s="66"/>
+      <c r="AM9" s="66"/>
+      <c r="AN9" s="66"/>
       <c r="AO9" s="18"/>
     </row>
     <row r="10" spans="1:41" ht="12.75">
       <c r="A10" s="6"/>
       <c r="B10" s="15"/>
-      <c r="C10" s="65"/>
-      <c r="D10" s="65"/>
-      <c r="E10" s="65"/>
-      <c r="F10" s="65"/>
-      <c r="G10" s="65"/>
-      <c r="H10" s="65"/>
-      <c r="I10" s="65"/>
-      <c r="J10" s="65"/>
-      <c r="K10" s="65"/>
-      <c r="L10" s="65"/>
-      <c r="M10" s="65"/>
-      <c r="N10" s="65"/>
-      <c r="O10" s="65"/>
-      <c r="P10" s="65"/>
-      <c r="Q10" s="65"/>
-      <c r="R10" s="65"/>
-      <c r="S10" s="65"/>
-      <c r="T10" s="65"/>
+      <c r="C10" s="66"/>
+      <c r="D10" s="66"/>
+      <c r="E10" s="66"/>
+      <c r="F10" s="66"/>
+      <c r="G10" s="66"/>
+      <c r="H10" s="66"/>
+      <c r="I10" s="66"/>
+      <c r="J10" s="66"/>
+      <c r="K10" s="66"/>
+      <c r="L10" s="66"/>
+      <c r="M10" s="66"/>
+      <c r="N10" s="66"/>
+      <c r="O10" s="66"/>
+      <c r="P10" s="66"/>
+      <c r="Q10" s="66"/>
+      <c r="R10" s="66"/>
+      <c r="S10" s="66"/>
+      <c r="T10" s="66"/>
       <c r="U10" s="17"/>
       <c r="V10" s="15"/>
-      <c r="W10" s="65"/>
-      <c r="X10" s="65"/>
-      <c r="Y10" s="65"/>
-      <c r="Z10" s="65"/>
-      <c r="AA10" s="65"/>
-      <c r="AB10" s="65"/>
-      <c r="AC10" s="65"/>
-      <c r="AD10" s="65"/>
-      <c r="AE10" s="65"/>
-      <c r="AF10" s="65"/>
-      <c r="AG10" s="65"/>
-      <c r="AH10" s="65"/>
-      <c r="AI10" s="65"/>
-      <c r="AJ10" s="65"/>
-      <c r="AK10" s="65"/>
-      <c r="AL10" s="65"/>
-      <c r="AM10" s="65"/>
-      <c r="AN10" s="65"/>
+      <c r="W10" s="66"/>
+      <c r="X10" s="66"/>
+      <c r="Y10" s="66"/>
+      <c r="Z10" s="66"/>
+      <c r="AA10" s="66"/>
+      <c r="AB10" s="66"/>
+      <c r="AC10" s="66"/>
+      <c r="AD10" s="66"/>
+      <c r="AE10" s="66"/>
+      <c r="AF10" s="66"/>
+      <c r="AG10" s="66"/>
+      <c r="AH10" s="66"/>
+      <c r="AI10" s="66"/>
+      <c r="AJ10" s="66"/>
+      <c r="AK10" s="66"/>
+      <c r="AL10" s="66"/>
+      <c r="AM10" s="66"/>
+      <c r="AN10" s="66"/>
       <c r="AO10" s="18"/>
     </row>
     <row r="11" spans="1:41" ht="12.75">
       <c r="A11" s="6"/>
       <c r="B11" s="15"/>
-      <c r="C11" s="65"/>
-      <c r="D11" s="65"/>
-      <c r="E11" s="65"/>
-      <c r="F11" s="65"/>
-      <c r="G11" s="65"/>
-      <c r="H11" s="65"/>
-      <c r="I11" s="65"/>
-      <c r="J11" s="65"/>
-      <c r="K11" s="65"/>
-      <c r="L11" s="65"/>
-      <c r="M11" s="65"/>
-      <c r="N11" s="65"/>
-      <c r="O11" s="65"/>
-      <c r="P11" s="65"/>
-      <c r="Q11" s="65"/>
-      <c r="R11" s="65"/>
-      <c r="S11" s="65"/>
-      <c r="T11" s="65"/>
+      <c r="C11" s="66"/>
+      <c r="D11" s="66"/>
+      <c r="E11" s="66"/>
+      <c r="F11" s="66"/>
+      <c r="G11" s="66"/>
+      <c r="H11" s="66"/>
+      <c r="I11" s="66"/>
+      <c r="J11" s="66"/>
+      <c r="K11" s="66"/>
+      <c r="L11" s="66"/>
+      <c r="M11" s="66"/>
+      <c r="N11" s="66"/>
+      <c r="O11" s="66"/>
+      <c r="P11" s="66"/>
+      <c r="Q11" s="66"/>
+      <c r="R11" s="66"/>
+      <c r="S11" s="66"/>
+      <c r="T11" s="66"/>
       <c r="U11" s="17"/>
       <c r="V11" s="15"/>
-      <c r="W11" s="65"/>
-      <c r="X11" s="65"/>
-      <c r="Y11" s="65"/>
-      <c r="Z11" s="65"/>
-      <c r="AA11" s="65"/>
-      <c r="AB11" s="65"/>
-      <c r="AC11" s="65"/>
-      <c r="AD11" s="65"/>
-      <c r="AE11" s="65"/>
-      <c r="AF11" s="65"/>
-      <c r="AG11" s="65"/>
-      <c r="AH11" s="65"/>
-      <c r="AI11" s="65"/>
-      <c r="AJ11" s="65"/>
-      <c r="AK11" s="65"/>
-      <c r="AL11" s="65"/>
-      <c r="AM11" s="65"/>
-      <c r="AN11" s="65"/>
+      <c r="W11" s="66"/>
+      <c r="X11" s="66"/>
+      <c r="Y11" s="66"/>
+      <c r="Z11" s="66"/>
+      <c r="AA11" s="66"/>
+      <c r="AB11" s="66"/>
+      <c r="AC11" s="66"/>
+      <c r="AD11" s="66"/>
+      <c r="AE11" s="66"/>
+      <c r="AF11" s="66"/>
+      <c r="AG11" s="66"/>
+      <c r="AH11" s="66"/>
+      <c r="AI11" s="66"/>
+      <c r="AJ11" s="66"/>
+      <c r="AK11" s="66"/>
+      <c r="AL11" s="66"/>
+      <c r="AM11" s="66"/>
+      <c r="AN11" s="66"/>
       <c r="AO11" s="18"/>
     </row>
     <row r="12" spans="1:41" ht="12.75">
       <c r="A12" s="6"/>
       <c r="B12" s="15"/>
-      <c r="C12" s="65"/>
-      <c r="D12" s="65"/>
-      <c r="E12" s="65"/>
-      <c r="F12" s="65"/>
-      <c r="G12" s="65"/>
-      <c r="H12" s="65"/>
-      <c r="I12" s="65"/>
-      <c r="J12" s="65"/>
-      <c r="K12" s="65"/>
-      <c r="L12" s="65"/>
-      <c r="M12" s="65"/>
-      <c r="N12" s="65"/>
-      <c r="O12" s="65"/>
-      <c r="P12" s="65"/>
-      <c r="Q12" s="65"/>
-      <c r="R12" s="65"/>
-      <c r="S12" s="65"/>
-      <c r="T12" s="65"/>
+      <c r="C12" s="66"/>
+      <c r="D12" s="66"/>
+      <c r="E12" s="66"/>
+      <c r="F12" s="66"/>
+      <c r="G12" s="66"/>
+      <c r="H12" s="66"/>
+      <c r="I12" s="66"/>
+      <c r="J12" s="66"/>
+      <c r="K12" s="66"/>
+      <c r="L12" s="66"/>
+      <c r="M12" s="66"/>
+      <c r="N12" s="66"/>
+      <c r="O12" s="66"/>
+      <c r="P12" s="66"/>
+      <c r="Q12" s="66"/>
+      <c r="R12" s="66"/>
+      <c r="S12" s="66"/>
+      <c r="T12" s="66"/>
       <c r="U12" s="17"/>
       <c r="V12" s="15"/>
-      <c r="W12" s="65"/>
-      <c r="X12" s="65"/>
-      <c r="Y12" s="65"/>
-      <c r="Z12" s="65"/>
-      <c r="AA12" s="65"/>
-      <c r="AB12" s="65"/>
-      <c r="AC12" s="65"/>
-      <c r="AD12" s="65"/>
-      <c r="AE12" s="65"/>
-      <c r="AF12" s="65"/>
-      <c r="AG12" s="65"/>
-      <c r="AH12" s="65"/>
-      <c r="AI12" s="65"/>
-      <c r="AJ12" s="65"/>
-      <c r="AK12" s="65"/>
-      <c r="AL12" s="65"/>
-      <c r="AM12" s="65"/>
-      <c r="AN12" s="65"/>
+      <c r="W12" s="66"/>
+      <c r="X12" s="66"/>
+      <c r="Y12" s="66"/>
+      <c r="Z12" s="66"/>
+      <c r="AA12" s="66"/>
+      <c r="AB12" s="66"/>
+      <c r="AC12" s="66"/>
+      <c r="AD12" s="66"/>
+      <c r="AE12" s="66"/>
+      <c r="AF12" s="66"/>
+      <c r="AG12" s="66"/>
+      <c r="AH12" s="66"/>
+      <c r="AI12" s="66"/>
+      <c r="AJ12" s="66"/>
+      <c r="AK12" s="66"/>
+      <c r="AL12" s="66"/>
+      <c r="AM12" s="66"/>
+      <c r="AN12" s="66"/>
       <c r="AO12" s="18"/>
     </row>
     <row r="13" spans="1:41" ht="12.75">
       <c r="A13" s="6"/>
       <c r="B13" s="15"/>
-      <c r="C13" s="65"/>
-      <c r="D13" s="65"/>
-      <c r="E13" s="65"/>
-      <c r="F13" s="65"/>
-      <c r="G13" s="65"/>
-      <c r="H13" s="65"/>
-      <c r="I13" s="65"/>
-      <c r="J13" s="65"/>
-      <c r="K13" s="65"/>
-      <c r="L13" s="65"/>
-      <c r="M13" s="65"/>
-      <c r="N13" s="65"/>
-      <c r="O13" s="65"/>
-      <c r="P13" s="65"/>
-      <c r="Q13" s="65"/>
-      <c r="R13" s="65"/>
-      <c r="S13" s="65"/>
-      <c r="T13" s="65"/>
+      <c r="C13" s="66"/>
+      <c r="D13" s="66"/>
+      <c r="E13" s="66"/>
+      <c r="F13" s="66"/>
+      <c r="G13" s="66"/>
+      <c r="H13" s="66"/>
+      <c r="I13" s="66"/>
+      <c r="J13" s="66"/>
+      <c r="K13" s="66"/>
+      <c r="L13" s="66"/>
+      <c r="M13" s="66"/>
+      <c r="N13" s="66"/>
+      <c r="O13" s="66"/>
+      <c r="P13" s="66"/>
+      <c r="Q13" s="66"/>
+      <c r="R13" s="66"/>
+      <c r="S13" s="66"/>
+      <c r="T13" s="66"/>
       <c r="U13" s="17"/>
       <c r="V13" s="15"/>
-      <c r="W13" s="65"/>
-      <c r="X13" s="65"/>
-      <c r="Y13" s="65"/>
-      <c r="Z13" s="65"/>
-      <c r="AA13" s="65"/>
-      <c r="AB13" s="65"/>
-      <c r="AC13" s="65"/>
-      <c r="AD13" s="65"/>
-      <c r="AE13" s="65"/>
-      <c r="AF13" s="65"/>
-      <c r="AG13" s="65"/>
-      <c r="AH13" s="65"/>
-      <c r="AI13" s="65"/>
-      <c r="AJ13" s="65"/>
-      <c r="AK13" s="65"/>
-      <c r="AL13" s="65"/>
-      <c r="AM13" s="65"/>
-      <c r="AN13" s="65"/>
+      <c r="W13" s="66"/>
+      <c r="X13" s="66"/>
+      <c r="Y13" s="66"/>
+      <c r="Z13" s="66"/>
+      <c r="AA13" s="66"/>
+      <c r="AB13" s="66"/>
+      <c r="AC13" s="66"/>
+      <c r="AD13" s="66"/>
+      <c r="AE13" s="66"/>
+      <c r="AF13" s="66"/>
+      <c r="AG13" s="66"/>
+      <c r="AH13" s="66"/>
+      <c r="AI13" s="66"/>
+      <c r="AJ13" s="66"/>
+      <c r="AK13" s="66"/>
+      <c r="AL13" s="66"/>
+      <c r="AM13" s="66"/>
+      <c r="AN13" s="66"/>
       <c r="AO13" s="18"/>
     </row>
     <row r="14" spans="1:41" ht="12.75">
@@ -2147,17 +2166,17 @@
       <c r="AB16" s="17" t="s">
         <v>40</v>
       </c>
-      <c r="AC16" s="66">
+      <c r="AC16" s="67">
         <v>47900266</v>
       </c>
-      <c r="AD16" s="66"/>
-      <c r="AE16" s="66"/>
-      <c r="AF16" s="66"/>
-      <c r="AG16" s="66"/>
-      <c r="AH16" s="66"/>
-      <c r="AI16" s="66"/>
-      <c r="AJ16" s="66"/>
-      <c r="AK16" s="66"/>
+      <c r="AD16" s="67"/>
+      <c r="AE16" s="67"/>
+      <c r="AF16" s="67"/>
+      <c r="AG16" s="67"/>
+      <c r="AH16" s="67"/>
+      <c r="AI16" s="67"/>
+      <c r="AJ16" s="67"/>
+      <c r="AK16" s="67"/>
       <c r="AL16" s="17"/>
       <c r="AM16" s="17"/>
       <c r="AN16" s="17"/>
@@ -2166,11 +2185,11 @@
     <row r="17" spans="1:41" ht="15">
       <c r="A17" s="6"/>
       <c r="B17" s="15"/>
-      <c r="C17" s="63" t="s">
+      <c r="C17" s="64" t="s">
         <v>41</v>
       </c>
-      <c r="D17" s="63"/>
-      <c r="E17" s="63"/>
+      <c r="D17" s="64"/>
+      <c r="E17" s="64"/>
       <c r="F17" s="23"/>
       <c r="G17" s="23"/>
       <c r="H17" s="23"/>
@@ -2198,17 +2217,17 @@
       <c r="AB17" s="17" t="s">
         <v>40</v>
       </c>
-      <c r="AC17" s="67">
+      <c r="AC17" s="68">
         <v>41865</v>
       </c>
-      <c r="AD17" s="67"/>
-      <c r="AE17" s="67"/>
-      <c r="AF17" s="67"/>
-      <c r="AG17" s="67"/>
-      <c r="AH17" s="67"/>
-      <c r="AI17" s="67"/>
-      <c r="AJ17" s="67"/>
-      <c r="AK17" s="67"/>
+      <c r="AD17" s="68"/>
+      <c r="AE17" s="68"/>
+      <c r="AF17" s="68"/>
+      <c r="AG17" s="68"/>
+      <c r="AH17" s="68"/>
+      <c r="AI17" s="68"/>
+      <c r="AJ17" s="68"/>
+      <c r="AK17" s="68"/>
       <c r="AL17" s="17"/>
       <c r="AM17" s="17"/>
       <c r="AN17" s="17"/>
@@ -2217,26 +2236,26 @@
     <row r="18" spans="1:41" ht="12.75">
       <c r="A18" s="6"/>
       <c r="B18" s="15"/>
-      <c r="C18" s="68" t="s">
+      <c r="C18" s="69" t="s">
         <v>43</v>
       </c>
-      <c r="D18" s="68"/>
-      <c r="E18" s="68"/>
-      <c r="F18" s="68"/>
-      <c r="G18" s="68"/>
-      <c r="H18" s="68"/>
-      <c r="I18" s="68"/>
-      <c r="J18" s="68"/>
-      <c r="K18" s="68"/>
-      <c r="L18" s="68"/>
-      <c r="M18" s="68"/>
-      <c r="N18" s="68"/>
-      <c r="O18" s="68"/>
-      <c r="P18" s="68"/>
-      <c r="Q18" s="68"/>
-      <c r="R18" s="68"/>
-      <c r="S18" s="68"/>
-      <c r="T18" s="68"/>
+      <c r="D18" s="69"/>
+      <c r="E18" s="69"/>
+      <c r="F18" s="69"/>
+      <c r="G18" s="69"/>
+      <c r="H18" s="69"/>
+      <c r="I18" s="69"/>
+      <c r="J18" s="69"/>
+      <c r="K18" s="69"/>
+      <c r="L18" s="69"/>
+      <c r="M18" s="69"/>
+      <c r="N18" s="69"/>
+      <c r="O18" s="69"/>
+      <c r="P18" s="69"/>
+      <c r="Q18" s="69"/>
+      <c r="R18" s="69"/>
+      <c r="S18" s="69"/>
+      <c r="T18" s="69"/>
       <c r="U18" s="18"/>
       <c r="V18" s="15"/>
       <c r="W18" s="17" t="s">
@@ -2249,17 +2268,17 @@
       <c r="AB18" s="17" t="s">
         <v>40</v>
       </c>
-      <c r="AC18" s="57" t="s">
+      <c r="AC18" s="58" t="s">
         <v>45</v>
       </c>
-      <c r="AD18" s="57"/>
-      <c r="AE18" s="57"/>
-      <c r="AF18" s="57"/>
-      <c r="AG18" s="57"/>
-      <c r="AH18" s="57"/>
-      <c r="AI18" s="57"/>
-      <c r="AJ18" s="57"/>
-      <c r="AK18" s="57"/>
+      <c r="AD18" s="58"/>
+      <c r="AE18" s="58"/>
+      <c r="AF18" s="58"/>
+      <c r="AG18" s="58"/>
+      <c r="AH18" s="58"/>
+      <c r="AI18" s="58"/>
+      <c r="AJ18" s="58"/>
+      <c r="AK18" s="58"/>
       <c r="AL18" s="17"/>
       <c r="AM18" s="17"/>
       <c r="AN18" s="17"/>
@@ -2268,24 +2287,24 @@
     <row r="19" spans="1:41" ht="12.75">
       <c r="A19" s="6"/>
       <c r="B19" s="15"/>
-      <c r="C19" s="68"/>
-      <c r="D19" s="68"/>
-      <c r="E19" s="68"/>
-      <c r="F19" s="68"/>
-      <c r="G19" s="68"/>
-      <c r="H19" s="68"/>
-      <c r="I19" s="68"/>
-      <c r="J19" s="68"/>
-      <c r="K19" s="68"/>
-      <c r="L19" s="68"/>
-      <c r="M19" s="68"/>
-      <c r="N19" s="68"/>
-      <c r="O19" s="68"/>
-      <c r="P19" s="68"/>
-      <c r="Q19" s="68"/>
-      <c r="R19" s="68"/>
-      <c r="S19" s="68"/>
-      <c r="T19" s="68"/>
+      <c r="C19" s="69"/>
+      <c r="D19" s="69"/>
+      <c r="E19" s="69"/>
+      <c r="F19" s="69"/>
+      <c r="G19" s="69"/>
+      <c r="H19" s="69"/>
+      <c r="I19" s="69"/>
+      <c r="J19" s="69"/>
+      <c r="K19" s="69"/>
+      <c r="L19" s="69"/>
+      <c r="M19" s="69"/>
+      <c r="N19" s="69"/>
+      <c r="O19" s="69"/>
+      <c r="P19" s="69"/>
+      <c r="Q19" s="69"/>
+      <c r="R19" s="69"/>
+      <c r="S19" s="69"/>
+      <c r="T19" s="69"/>
       <c r="U19" s="18"/>
       <c r="V19" s="15"/>
       <c r="W19" s="17" t="s">
@@ -2298,16 +2317,16 @@
       <c r="AB19" s="17" t="s">
         <v>40</v>
       </c>
-      <c r="AC19" s="57" t="s">
+      <c r="AC19" s="58" t="s">
         <v>47</v>
       </c>
-      <c r="AD19" s="57"/>
-      <c r="AE19" s="57"/>
-      <c r="AF19" s="57"/>
-      <c r="AG19" s="57"/>
-      <c r="AH19" s="57"/>
-      <c r="AI19" s="57"/>
-      <c r="AJ19" s="57"/>
+      <c r="AD19" s="58"/>
+      <c r="AE19" s="58"/>
+      <c r="AF19" s="58"/>
+      <c r="AG19" s="58"/>
+      <c r="AH19" s="58"/>
+      <c r="AI19" s="58"/>
+      <c r="AJ19" s="58"/>
       <c r="AK19" s="24"/>
       <c r="AL19" s="17"/>
       <c r="AM19" s="17"/>
@@ -2317,24 +2336,24 @@
     <row r="20" spans="1:41" ht="12.75">
       <c r="A20" s="6"/>
       <c r="B20" s="15"/>
-      <c r="C20" s="68"/>
-      <c r="D20" s="68"/>
-      <c r="E20" s="68"/>
-      <c r="F20" s="68"/>
-      <c r="G20" s="68"/>
-      <c r="H20" s="68"/>
-      <c r="I20" s="68"/>
-      <c r="J20" s="68"/>
-      <c r="K20" s="68"/>
-      <c r="L20" s="68"/>
-      <c r="M20" s="68"/>
-      <c r="N20" s="68"/>
-      <c r="O20" s="68"/>
-      <c r="P20" s="68"/>
-      <c r="Q20" s="68"/>
-      <c r="R20" s="68"/>
-      <c r="S20" s="68"/>
-      <c r="T20" s="68"/>
+      <c r="C20" s="69"/>
+      <c r="D20" s="69"/>
+      <c r="E20" s="69"/>
+      <c r="F20" s="69"/>
+      <c r="G20" s="69"/>
+      <c r="H20" s="69"/>
+      <c r="I20" s="69"/>
+      <c r="J20" s="69"/>
+      <c r="K20" s="69"/>
+      <c r="L20" s="69"/>
+      <c r="M20" s="69"/>
+      <c r="N20" s="69"/>
+      <c r="O20" s="69"/>
+      <c r="P20" s="69"/>
+      <c r="Q20" s="69"/>
+      <c r="R20" s="69"/>
+      <c r="S20" s="69"/>
+      <c r="T20" s="69"/>
       <c r="U20" s="18"/>
       <c r="V20" s="15"/>
       <c r="W20" s="17" t="s">
@@ -2347,17 +2366,17 @@
       <c r="AB20" s="17" t="s">
         <v>40</v>
       </c>
-      <c r="AC20" s="57" t="s">
+      <c r="AC20" s="58" t="s">
         <v>49</v>
       </c>
-      <c r="AD20" s="57"/>
-      <c r="AE20" s="57"/>
-      <c r="AF20" s="57"/>
-      <c r="AG20" s="57"/>
-      <c r="AH20" s="57"/>
-      <c r="AI20" s="57"/>
-      <c r="AJ20" s="57"/>
-      <c r="AK20" s="57"/>
+      <c r="AD20" s="58"/>
+      <c r="AE20" s="58"/>
+      <c r="AF20" s="58"/>
+      <c r="AG20" s="58"/>
+      <c r="AH20" s="58"/>
+      <c r="AI20" s="58"/>
+      <c r="AJ20" s="58"/>
+      <c r="AK20" s="58"/>
       <c r="AL20" s="17"/>
       <c r="AM20" s="17"/>
       <c r="AN20" s="17"/>
@@ -2366,24 +2385,24 @@
     <row r="21" spans="1:41" ht="12.75">
       <c r="A21" s="6"/>
       <c r="B21" s="15"/>
-      <c r="C21" s="68"/>
-      <c r="D21" s="68"/>
-      <c r="E21" s="68"/>
-      <c r="F21" s="68"/>
-      <c r="G21" s="68"/>
-      <c r="H21" s="68"/>
-      <c r="I21" s="68"/>
-      <c r="J21" s="68"/>
-      <c r="K21" s="68"/>
-      <c r="L21" s="68"/>
-      <c r="M21" s="68"/>
-      <c r="N21" s="68"/>
-      <c r="O21" s="68"/>
-      <c r="P21" s="68"/>
-      <c r="Q21" s="68"/>
-      <c r="R21" s="68"/>
-      <c r="S21" s="68"/>
-      <c r="T21" s="68"/>
+      <c r="C21" s="69"/>
+      <c r="D21" s="69"/>
+      <c r="E21" s="69"/>
+      <c r="F21" s="69"/>
+      <c r="G21" s="69"/>
+      <c r="H21" s="69"/>
+      <c r="I21" s="69"/>
+      <c r="J21" s="69"/>
+      <c r="K21" s="69"/>
+      <c r="L21" s="69"/>
+      <c r="M21" s="69"/>
+      <c r="N21" s="69"/>
+      <c r="O21" s="69"/>
+      <c r="P21" s="69"/>
+      <c r="Q21" s="69"/>
+      <c r="R21" s="69"/>
+      <c r="S21" s="69"/>
+      <c r="T21" s="69"/>
       <c r="U21" s="18"/>
       <c r="V21" s="15"/>
       <c r="W21" s="17"/>
@@ -2392,12 +2411,12 @@
       <c r="Z21" s="17"/>
       <c r="AA21" s="17"/>
       <c r="AB21" s="17"/>
-      <c r="AC21" s="57"/>
-      <c r="AD21" s="57"/>
-      <c r="AE21" s="57"/>
-      <c r="AF21" s="57"/>
-      <c r="AG21" s="57"/>
-      <c r="AH21" s="57"/>
+      <c r="AC21" s="58"/>
+      <c r="AD21" s="58"/>
+      <c r="AE21" s="58"/>
+      <c r="AF21" s="58"/>
+      <c r="AG21" s="58"/>
+      <c r="AH21" s="58"/>
       <c r="AI21" s="17"/>
       <c r="AJ21" s="17"/>
       <c r="AK21" s="17"/>
@@ -2409,24 +2428,24 @@
     <row r="22" spans="1:41" ht="15">
       <c r="A22" s="6"/>
       <c r="B22" s="15"/>
-      <c r="C22" s="63"/>
-      <c r="D22" s="63"/>
-      <c r="E22" s="63"/>
-      <c r="F22" s="63"/>
-      <c r="G22" s="63"/>
-      <c r="H22" s="63"/>
-      <c r="I22" s="63"/>
-      <c r="J22" s="63"/>
-      <c r="K22" s="63"/>
-      <c r="L22" s="63"/>
-      <c r="M22" s="63"/>
-      <c r="N22" s="63"/>
-      <c r="O22" s="63"/>
-      <c r="P22" s="63"/>
-      <c r="Q22" s="63"/>
-      <c r="R22" s="63"/>
-      <c r="S22" s="63"/>
-      <c r="T22" s="63"/>
+      <c r="C22" s="64"/>
+      <c r="D22" s="64"/>
+      <c r="E22" s="64"/>
+      <c r="F22" s="64"/>
+      <c r="G22" s="64"/>
+      <c r="H22" s="64"/>
+      <c r="I22" s="64"/>
+      <c r="J22" s="64"/>
+      <c r="K22" s="64"/>
+      <c r="L22" s="64"/>
+      <c r="M22" s="64"/>
+      <c r="N22" s="64"/>
+      <c r="O22" s="64"/>
+      <c r="P22" s="64"/>
+      <c r="Q22" s="64"/>
+      <c r="R22" s="64"/>
+      <c r="S22" s="64"/>
+      <c r="T22" s="64"/>
       <c r="U22" s="18"/>
       <c r="V22" s="15"/>
       <c r="W22" s="17"/>
@@ -2435,12 +2454,12 @@
       <c r="Z22" s="17"/>
       <c r="AA22" s="17"/>
       <c r="AB22" s="17"/>
-      <c r="AC22" s="57"/>
-      <c r="AD22" s="57"/>
-      <c r="AE22" s="57"/>
-      <c r="AF22" s="57"/>
-      <c r="AG22" s="57"/>
-      <c r="AH22" s="57"/>
+      <c r="AC22" s="58"/>
+      <c r="AD22" s="58"/>
+      <c r="AE22" s="58"/>
+      <c r="AF22" s="58"/>
+      <c r="AG22" s="58"/>
+      <c r="AH22" s="58"/>
       <c r="AI22" s="17"/>
       <c r="AJ22" s="17"/>
       <c r="AK22" s="17"/>
@@ -2530,115 +2549,115 @@
       <c r="AI24" s="13"/>
       <c r="AJ24" s="13"/>
       <c r="AK24" s="13"/>
-      <c r="AL24" s="58" t="s">
+      <c r="AL24" s="59" t="s">
         <v>50</v>
       </c>
-      <c r="AM24" s="58"/>
-      <c r="AN24" s="58"/>
+      <c r="AM24" s="59"/>
+      <c r="AN24" s="59"/>
       <c r="AO24" s="14"/>
     </row>
     <row r="25" spans="1:41" ht="12.75">
       <c r="A25" s="6"/>
       <c r="B25" s="15"/>
-      <c r="C25" s="59" t="s">
+      <c r="C25" s="60" t="s">
         <v>51</v>
       </c>
-      <c r="D25" s="59"/>
-      <c r="E25" s="59"/>
-      <c r="F25" s="59"/>
+      <c r="D25" s="60"/>
+      <c r="E25" s="60"/>
+      <c r="F25" s="60"/>
       <c r="G25" s="25"/>
-      <c r="H25" s="60" t="s">
+      <c r="H25" s="61" t="s">
         <v>52</v>
       </c>
-      <c r="I25" s="60"/>
-      <c r="J25" s="60"/>
+      <c r="I25" s="61"/>
+      <c r="J25" s="61"/>
       <c r="K25" s="25"/>
-      <c r="L25" s="61" t="s">
+      <c r="L25" s="62" t="s">
         <v>53</v>
       </c>
-      <c r="M25" s="61"/>
-      <c r="N25" s="61"/>
-      <c r="O25" s="61"/>
-      <c r="P25" s="61"/>
+      <c r="M25" s="62"/>
+      <c r="N25" s="62"/>
+      <c r="O25" s="62"/>
+      <c r="P25" s="62"/>
       <c r="Q25" s="26"/>
-      <c r="R25" s="62" t="s">
+      <c r="R25" s="63" t="s">
         <v>54</v>
       </c>
-      <c r="S25" s="62"/>
-      <c r="T25" s="62"/>
-      <c r="U25" s="62"/>
-      <c r="V25" s="62"/>
-      <c r="W25" s="62"/>
-      <c r="X25" s="62"/>
-      <c r="Y25" s="62"/>
-      <c r="Z25" s="62"/>
-      <c r="AA25" s="62"/>
-      <c r="AB25" s="62"/>
-      <c r="AC25" s="62"/>
-      <c r="AD25" s="62"/>
-      <c r="AE25" s="62" t="s">
+      <c r="S25" s="63"/>
+      <c r="T25" s="63"/>
+      <c r="U25" s="63"/>
+      <c r="V25" s="63"/>
+      <c r="W25" s="63"/>
+      <c r="X25" s="63"/>
+      <c r="Y25" s="63"/>
+      <c r="Z25" s="63"/>
+      <c r="AA25" s="63"/>
+      <c r="AB25" s="63"/>
+      <c r="AC25" s="63"/>
+      <c r="AD25" s="63"/>
+      <c r="AE25" s="63" t="s">
         <v>55</v>
       </c>
-      <c r="AF25" s="62"/>
+      <c r="AF25" s="63"/>
       <c r="AG25" s="25"/>
-      <c r="AH25" s="59" t="str">
+      <c r="AH25" s="60" t="str">
         <f>CONCATENATE("UNIT PRICE",CHAR(10),"(",AL24,")")</f>
         <v>UNIT PRICE
 (SGD)</v>
       </c>
-      <c r="AI25" s="59"/>
-      <c r="AJ25" s="59"/>
+      <c r="AI25" s="60"/>
+      <c r="AJ25" s="60"/>
       <c r="AK25" s="25"/>
-      <c r="AL25" s="59" t="str">
+      <c r="AL25" s="60" t="str">
         <f>CONCATENATE("TOTAL",CHAR(10),"(",AL24,")")</f>
         <v>TOTAL
 (SGD)</v>
       </c>
-      <c r="AM25" s="59"/>
-      <c r="AN25" s="59"/>
+      <c r="AM25" s="60"/>
+      <c r="AN25" s="60"/>
       <c r="AO25" s="18"/>
     </row>
     <row r="26" spans="1:41" ht="12.75">
       <c r="A26" s="6"/>
       <c r="B26" s="15"/>
-      <c r="C26" s="59"/>
-      <c r="D26" s="59"/>
-      <c r="E26" s="59"/>
-      <c r="F26" s="59"/>
+      <c r="C26" s="60"/>
+      <c r="D26" s="60"/>
+      <c r="E26" s="60"/>
+      <c r="F26" s="60"/>
       <c r="G26" s="25"/>
-      <c r="H26" s="60"/>
-      <c r="I26" s="60"/>
-      <c r="J26" s="60"/>
+      <c r="H26" s="61"/>
+      <c r="I26" s="61"/>
+      <c r="J26" s="61"/>
       <c r="K26" s="25"/>
-      <c r="L26" s="61"/>
-      <c r="M26" s="61"/>
-      <c r="N26" s="61"/>
-      <c r="O26" s="61"/>
-      <c r="P26" s="61"/>
+      <c r="L26" s="62"/>
+      <c r="M26" s="62"/>
+      <c r="N26" s="62"/>
+      <c r="O26" s="62"/>
+      <c r="P26" s="62"/>
       <c r="Q26" s="26"/>
-      <c r="R26" s="62"/>
-      <c r="S26" s="62"/>
-      <c r="T26" s="62"/>
-      <c r="U26" s="62"/>
-      <c r="V26" s="62"/>
-      <c r="W26" s="62"/>
-      <c r="X26" s="62"/>
-      <c r="Y26" s="62"/>
-      <c r="Z26" s="62"/>
-      <c r="AA26" s="62"/>
-      <c r="AB26" s="62"/>
-      <c r="AC26" s="62"/>
-      <c r="AD26" s="62"/>
-      <c r="AE26" s="62"/>
-      <c r="AF26" s="62"/>
+      <c r="R26" s="63"/>
+      <c r="S26" s="63"/>
+      <c r="T26" s="63"/>
+      <c r="U26" s="63"/>
+      <c r="V26" s="63"/>
+      <c r="W26" s="63"/>
+      <c r="X26" s="63"/>
+      <c r="Y26" s="63"/>
+      <c r="Z26" s="63"/>
+      <c r="AA26" s="63"/>
+      <c r="AB26" s="63"/>
+      <c r="AC26" s="63"/>
+      <c r="AD26" s="63"/>
+      <c r="AE26" s="63"/>
+      <c r="AF26" s="63"/>
       <c r="AG26" s="25"/>
-      <c r="AH26" s="59"/>
-      <c r="AI26" s="59"/>
-      <c r="AJ26" s="59"/>
+      <c r="AH26" s="60"/>
+      <c r="AI26" s="60"/>
+      <c r="AJ26" s="60"/>
       <c r="AK26" s="25"/>
-      <c r="AL26" s="59"/>
-      <c r="AM26" s="59"/>
-      <c r="AN26" s="59"/>
+      <c r="AL26" s="60"/>
+      <c r="AM26" s="60"/>
+      <c r="AN26" s="60"/>
       <c r="AO26" s="18"/>
     </row>
     <row r="27" spans="1:41" ht="12.75">
@@ -2686,46 +2705,46 @@
     </row>
     <row r="28" spans="1:41" ht="12.75">
       <c r="A28" s="6"/>
-      <c r="B28" s="54"/>
-      <c r="C28" s="55"/>
-      <c r="D28" s="55"/>
-      <c r="E28" s="55"/>
-      <c r="F28" s="55"/>
-      <c r="G28" s="55"/>
-      <c r="H28" s="55"/>
-      <c r="I28" s="55"/>
-      <c r="J28" s="55"/>
-      <c r="K28" s="55"/>
-      <c r="L28" s="55"/>
-      <c r="M28" s="55"/>
-      <c r="N28" s="55"/>
-      <c r="O28" s="55"/>
-      <c r="P28" s="55"/>
-      <c r="Q28" s="55"/>
-      <c r="R28" s="55"/>
-      <c r="S28" s="55"/>
-      <c r="T28" s="55"/>
-      <c r="U28" s="55"/>
-      <c r="V28" s="55"/>
-      <c r="W28" s="55"/>
-      <c r="X28" s="55"/>
-      <c r="Y28" s="55"/>
-      <c r="Z28" s="55"/>
-      <c r="AA28" s="55"/>
-      <c r="AB28" s="55"/>
-      <c r="AC28" s="55"/>
-      <c r="AD28" s="55"/>
-      <c r="AE28" s="55"/>
-      <c r="AF28" s="55"/>
-      <c r="AG28" s="55"/>
-      <c r="AH28" s="55"/>
-      <c r="AI28" s="55"/>
-      <c r="AJ28" s="55"/>
-      <c r="AK28" s="55"/>
-      <c r="AL28" s="55"/>
-      <c r="AM28" s="55"/>
-      <c r="AN28" s="55"/>
-      <c r="AO28" s="56"/>
+      <c r="B28" s="55"/>
+      <c r="C28" s="56"/>
+      <c r="D28" s="56"/>
+      <c r="E28" s="56"/>
+      <c r="F28" s="56"/>
+      <c r="G28" s="56"/>
+      <c r="H28" s="56"/>
+      <c r="I28" s="56"/>
+      <c r="J28" s="56"/>
+      <c r="K28" s="56"/>
+      <c r="L28" s="56"/>
+      <c r="M28" s="56"/>
+      <c r="N28" s="56"/>
+      <c r="O28" s="56"/>
+      <c r="P28" s="56"/>
+      <c r="Q28" s="56"/>
+      <c r="R28" s="56"/>
+      <c r="S28" s="56"/>
+      <c r="T28" s="56"/>
+      <c r="U28" s="56"/>
+      <c r="V28" s="56"/>
+      <c r="W28" s="56"/>
+      <c r="X28" s="56"/>
+      <c r="Y28" s="56"/>
+      <c r="Z28" s="56"/>
+      <c r="AA28" s="56"/>
+      <c r="AB28" s="56"/>
+      <c r="AC28" s="56"/>
+      <c r="AD28" s="56"/>
+      <c r="AE28" s="56"/>
+      <c r="AF28" s="56"/>
+      <c r="AG28" s="56"/>
+      <c r="AH28" s="56"/>
+      <c r="AI28" s="56"/>
+      <c r="AJ28" s="56"/>
+      <c r="AK28" s="56"/>
+      <c r="AL28" s="56"/>
+      <c r="AM28" s="56"/>
+      <c r="AN28" s="56"/>
+      <c r="AO28" s="57"/>
     </row>
     <row r="29" spans="1:41" s="11" customFormat="1" ht="87.75" customHeight="1">
       <c r="A29" s="8"/>
@@ -2743,13 +2762,13 @@
       <c r="I29" s="51"/>
       <c r="J29" s="51"/>
       <c r="K29" s="29"/>
-      <c r="L29" s="76" t="s">
+      <c r="L29" s="54" t="s">
         <v>57</v>
       </c>
-      <c r="M29" s="76"/>
-      <c r="N29" s="76"/>
-      <c r="O29" s="76"/>
-      <c r="P29" s="76"/>
+      <c r="M29" s="54"/>
+      <c r="N29" s="54"/>
+      <c r="O29" s="54"/>
+      <c r="P29" s="54"/>
       <c r="Q29" s="30"/>
       <c r="R29" s="52" t="s">
         <v>58</v>
@@ -2801,13 +2820,13 @@
       <c r="I30" s="51"/>
       <c r="J30" s="51"/>
       <c r="K30" s="29"/>
-      <c r="L30" s="76" t="s">
+      <c r="L30" s="54" t="s">
         <v>57</v>
       </c>
-      <c r="M30" s="76"/>
-      <c r="N30" s="76"/>
-      <c r="O30" s="76"/>
-      <c r="P30" s="76"/>
+      <c r="M30" s="54"/>
+      <c r="N30" s="54"/>
+      <c r="O30" s="54"/>
+      <c r="P30" s="54"/>
       <c r="Q30" s="30"/>
       <c r="R30" s="52" t="s">
         <v>58</v>
@@ -2859,13 +2878,13 @@
       <c r="I31" s="51"/>
       <c r="J31" s="51"/>
       <c r="K31" s="29"/>
-      <c r="L31" s="76" t="s">
+      <c r="L31" s="54" t="s">
         <v>57</v>
       </c>
-      <c r="M31" s="76"/>
-      <c r="N31" s="76"/>
-      <c r="O31" s="76"/>
-      <c r="P31" s="76"/>
+      <c r="M31" s="54"/>
+      <c r="N31" s="54"/>
+      <c r="O31" s="54"/>
+      <c r="P31" s="54"/>
       <c r="Q31" s="30"/>
       <c r="R31" s="52" t="s">
         <v>58</v>
@@ -2917,13 +2936,13 @@
       <c r="I32" s="51"/>
       <c r="J32" s="51"/>
       <c r="K32" s="29"/>
-      <c r="L32" s="76" t="s">
+      <c r="L32" s="54" t="s">
         <v>57</v>
       </c>
-      <c r="M32" s="76"/>
-      <c r="N32" s="76"/>
-      <c r="O32" s="76"/>
-      <c r="P32" s="76"/>
+      <c r="M32" s="54"/>
+      <c r="N32" s="54"/>
+      <c r="O32" s="54"/>
+      <c r="P32" s="54"/>
       <c r="Q32" s="30"/>
       <c r="R32" s="52" t="s">
         <v>58</v>
@@ -2975,13 +2994,13 @@
       <c r="I33" s="51"/>
       <c r="J33" s="51"/>
       <c r="K33" s="29"/>
-      <c r="L33" s="76" t="s">
+      <c r="L33" s="54" t="s">
         <v>57</v>
       </c>
-      <c r="M33" s="76"/>
-      <c r="N33" s="76"/>
-      <c r="O33" s="76"/>
-      <c r="P33" s="76"/>
+      <c r="M33" s="54"/>
+      <c r="N33" s="54"/>
+      <c r="O33" s="54"/>
+      <c r="P33" s="54"/>
       <c r="Q33" s="30"/>
       <c r="R33" s="52" t="s">
         <v>58</v>

</xml_diff>

<commit_message>
Fix bugs with Copying Worksheet & Inserting Row.
Signed-off-by: gengxuehong <gengxuehong@foxmail.com>
</commit_message>
<xml_diff>
--- a/Develop/Giga/Giga.Test/Transformer/TransformerTest.xlsx
+++ b/Develop/Giga/Giga.Test/Transformer/TransformerTest.xlsx
@@ -630,6 +630,96 @@
     <xf numFmtId="0" fontId="11" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="179" fontId="3" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="179" fontId="3" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="4" fontId="3" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="3" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="3" fillId="3" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="14" fillId="7" borderId="8" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -653,96 +743,6 @@
     </xf>
     <xf numFmtId="0" fontId="14" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="3" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="3" fillId="3" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="179" fontId="3" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="4" fontId="3" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="179" fontId="3" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1097,7 +1097,7 @@
   <dimension ref="A1:J12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H12" sqref="H12"/>
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -1418,6 +1418,14 @@
     <row r="12" spans="1:10">
       <c r="A12" t="s">
         <v>28</v>
+      </c>
+      <c r="C12" t="str">
+        <f>CONCATENATE(C11,D11)</f>
+        <v>POS-9395-ADDFPOS Machine Part 008</v>
+      </c>
+      <c r="D12" t="str">
+        <f>D11</f>
+        <v>POS Machine Part 008</v>
       </c>
       <c r="E12" s="4">
         <f>SUM(E4:E11)</f>
@@ -1473,37 +1481,37 @@
       <c r="D1" s="6"/>
       <c r="E1" s="6"/>
       <c r="F1" s="6"/>
-      <c r="G1" s="71"/>
-      <c r="H1" s="71"/>
-      <c r="I1" s="71"/>
-      <c r="J1" s="71"/>
-      <c r="K1" s="71"/>
-      <c r="L1" s="71"/>
-      <c r="M1" s="71"/>
-      <c r="N1" s="71"/>
-      <c r="O1" s="71"/>
-      <c r="P1" s="71"/>
-      <c r="Q1" s="71"/>
-      <c r="R1" s="71"/>
-      <c r="S1" s="71"/>
-      <c r="T1" s="71"/>
-      <c r="U1" s="71"/>
-      <c r="V1" s="71"/>
-      <c r="W1" s="71"/>
-      <c r="X1" s="71"/>
-      <c r="Y1" s="71"/>
-      <c r="Z1" s="71"/>
-      <c r="AA1" s="71"/>
-      <c r="AB1" s="71"/>
-      <c r="AC1" s="71"/>
-      <c r="AD1" s="71"/>
-      <c r="AE1" s="71"/>
-      <c r="AF1" s="71"/>
-      <c r="AG1" s="71"/>
-      <c r="AH1" s="71"/>
-      <c r="AI1" s="71"/>
-      <c r="AJ1" s="71"/>
-      <c r="AK1" s="71"/>
+      <c r="G1" s="40"/>
+      <c r="H1" s="40"/>
+      <c r="I1" s="40"/>
+      <c r="J1" s="40"/>
+      <c r="K1" s="40"/>
+      <c r="L1" s="40"/>
+      <c r="M1" s="40"/>
+      <c r="N1" s="40"/>
+      <c r="O1" s="40"/>
+      <c r="P1" s="40"/>
+      <c r="Q1" s="40"/>
+      <c r="R1" s="40"/>
+      <c r="S1" s="40"/>
+      <c r="T1" s="40"/>
+      <c r="U1" s="40"/>
+      <c r="V1" s="40"/>
+      <c r="W1" s="40"/>
+      <c r="X1" s="40"/>
+      <c r="Y1" s="40"/>
+      <c r="Z1" s="40"/>
+      <c r="AA1" s="40"/>
+      <c r="AB1" s="40"/>
+      <c r="AC1" s="40"/>
+      <c r="AD1" s="40"/>
+      <c r="AE1" s="40"/>
+      <c r="AF1" s="40"/>
+      <c r="AG1" s="40"/>
+      <c r="AH1" s="40"/>
+      <c r="AI1" s="40"/>
+      <c r="AJ1" s="40"/>
+      <c r="AK1" s="40"/>
       <c r="AL1" s="6"/>
       <c r="AM1" s="6"/>
       <c r="AN1" s="6"/>
@@ -1516,40 +1524,40 @@
       <c r="D2" s="6"/>
       <c r="E2" s="6"/>
       <c r="F2" s="6"/>
-      <c r="G2" s="72" t="s">
+      <c r="G2" s="41" t="s">
         <v>29</v>
       </c>
-      <c r="H2" s="73"/>
-      <c r="I2" s="73"/>
-      <c r="J2" s="73"/>
-      <c r="K2" s="73"/>
-      <c r="L2" s="73"/>
-      <c r="M2" s="73"/>
-      <c r="N2" s="73"/>
-      <c r="O2" s="73"/>
-      <c r="P2" s="73"/>
-      <c r="Q2" s="73"/>
-      <c r="R2" s="73"/>
-      <c r="S2" s="73"/>
-      <c r="T2" s="73"/>
-      <c r="U2" s="73"/>
-      <c r="V2" s="73"/>
-      <c r="W2" s="73"/>
-      <c r="X2" s="73"/>
-      <c r="Y2" s="73"/>
-      <c r="Z2" s="73"/>
-      <c r="AA2" s="73"/>
-      <c r="AB2" s="73"/>
-      <c r="AC2" s="73"/>
-      <c r="AD2" s="73"/>
-      <c r="AE2" s="73"/>
-      <c r="AF2" s="73"/>
-      <c r="AG2" s="73"/>
-      <c r="AH2" s="73"/>
-      <c r="AI2" s="73"/>
-      <c r="AJ2" s="73"/>
-      <c r="AK2" s="73"/>
-      <c r="AL2" s="73"/>
+      <c r="H2" s="42"/>
+      <c r="I2" s="42"/>
+      <c r="J2" s="42"/>
+      <c r="K2" s="42"/>
+      <c r="L2" s="42"/>
+      <c r="M2" s="42"/>
+      <c r="N2" s="42"/>
+      <c r="O2" s="42"/>
+      <c r="P2" s="42"/>
+      <c r="Q2" s="42"/>
+      <c r="R2" s="42"/>
+      <c r="S2" s="42"/>
+      <c r="T2" s="42"/>
+      <c r="U2" s="42"/>
+      <c r="V2" s="42"/>
+      <c r="W2" s="42"/>
+      <c r="X2" s="42"/>
+      <c r="Y2" s="42"/>
+      <c r="Z2" s="42"/>
+      <c r="AA2" s="42"/>
+      <c r="AB2" s="42"/>
+      <c r="AC2" s="42"/>
+      <c r="AD2" s="42"/>
+      <c r="AE2" s="42"/>
+      <c r="AF2" s="42"/>
+      <c r="AG2" s="42"/>
+      <c r="AH2" s="42"/>
+      <c r="AI2" s="42"/>
+      <c r="AJ2" s="42"/>
+      <c r="AK2" s="42"/>
+      <c r="AL2" s="42"/>
       <c r="AM2" s="6"/>
       <c r="AN2" s="6"/>
       <c r="AO2" s="6"/>
@@ -1561,40 +1569,40 @@
       <c r="D3" s="6"/>
       <c r="E3" s="6"/>
       <c r="F3" s="6"/>
-      <c r="G3" s="71" t="s">
+      <c r="G3" s="40" t="s">
         <v>30</v>
       </c>
-      <c r="H3" s="71"/>
-      <c r="I3" s="71"/>
-      <c r="J3" s="71"/>
-      <c r="K3" s="71"/>
-      <c r="L3" s="71"/>
-      <c r="M3" s="71"/>
-      <c r="N3" s="71"/>
-      <c r="O3" s="71"/>
-      <c r="P3" s="71"/>
-      <c r="Q3" s="71"/>
-      <c r="R3" s="71"/>
-      <c r="S3" s="71"/>
-      <c r="T3" s="71"/>
-      <c r="U3" s="71"/>
-      <c r="V3" s="71"/>
-      <c r="W3" s="71"/>
-      <c r="X3" s="71"/>
-      <c r="Y3" s="71"/>
-      <c r="Z3" s="71"/>
-      <c r="AA3" s="71"/>
-      <c r="AB3" s="71"/>
-      <c r="AC3" s="71"/>
-      <c r="AD3" s="71"/>
-      <c r="AE3" s="71"/>
-      <c r="AF3" s="71"/>
-      <c r="AG3" s="71"/>
-      <c r="AH3" s="71"/>
-      <c r="AI3" s="71"/>
-      <c r="AJ3" s="71"/>
-      <c r="AK3" s="71"/>
-      <c r="AL3" s="71"/>
+      <c r="H3" s="40"/>
+      <c r="I3" s="40"/>
+      <c r="J3" s="40"/>
+      <c r="K3" s="40"/>
+      <c r="L3" s="40"/>
+      <c r="M3" s="40"/>
+      <c r="N3" s="40"/>
+      <c r="O3" s="40"/>
+      <c r="P3" s="40"/>
+      <c r="Q3" s="40"/>
+      <c r="R3" s="40"/>
+      <c r="S3" s="40"/>
+      <c r="T3" s="40"/>
+      <c r="U3" s="40"/>
+      <c r="V3" s="40"/>
+      <c r="W3" s="40"/>
+      <c r="X3" s="40"/>
+      <c r="Y3" s="40"/>
+      <c r="Z3" s="40"/>
+      <c r="AA3" s="40"/>
+      <c r="AB3" s="40"/>
+      <c r="AC3" s="40"/>
+      <c r="AD3" s="40"/>
+      <c r="AE3" s="40"/>
+      <c r="AF3" s="40"/>
+      <c r="AG3" s="40"/>
+      <c r="AH3" s="40"/>
+      <c r="AI3" s="40"/>
+      <c r="AJ3" s="40"/>
+      <c r="AK3" s="40"/>
+      <c r="AL3" s="40"/>
       <c r="AM3" s="6"/>
       <c r="AN3" s="6"/>
       <c r="AO3" s="6"/>
@@ -1606,40 +1614,40 @@
       <c r="D4" s="6"/>
       <c r="E4" s="6"/>
       <c r="F4" s="6"/>
-      <c r="G4" s="74" t="s">
+      <c r="G4" s="43" t="s">
         <v>31</v>
       </c>
-      <c r="H4" s="74"/>
-      <c r="I4" s="74"/>
-      <c r="J4" s="74"/>
-      <c r="K4" s="74"/>
-      <c r="L4" s="74"/>
-      <c r="M4" s="74"/>
-      <c r="N4" s="74"/>
-      <c r="O4" s="74"/>
-      <c r="P4" s="74"/>
-      <c r="Q4" s="74"/>
-      <c r="R4" s="74"/>
-      <c r="S4" s="74"/>
-      <c r="T4" s="74"/>
-      <c r="U4" s="74"/>
-      <c r="V4" s="74"/>
-      <c r="W4" s="74"/>
-      <c r="X4" s="74"/>
-      <c r="Y4" s="74"/>
-      <c r="Z4" s="74"/>
-      <c r="AA4" s="74"/>
-      <c r="AB4" s="74"/>
-      <c r="AC4" s="74"/>
-      <c r="AD4" s="74"/>
-      <c r="AE4" s="74"/>
-      <c r="AF4" s="74"/>
-      <c r="AG4" s="74"/>
-      <c r="AH4" s="74"/>
-      <c r="AI4" s="74"/>
-      <c r="AJ4" s="74"/>
-      <c r="AK4" s="74"/>
-      <c r="AL4" s="74"/>
+      <c r="H4" s="43"/>
+      <c r="I4" s="43"/>
+      <c r="J4" s="43"/>
+      <c r="K4" s="43"/>
+      <c r="L4" s="43"/>
+      <c r="M4" s="43"/>
+      <c r="N4" s="43"/>
+      <c r="O4" s="43"/>
+      <c r="P4" s="43"/>
+      <c r="Q4" s="43"/>
+      <c r="R4" s="43"/>
+      <c r="S4" s="43"/>
+      <c r="T4" s="43"/>
+      <c r="U4" s="43"/>
+      <c r="V4" s="43"/>
+      <c r="W4" s="43"/>
+      <c r="X4" s="43"/>
+      <c r="Y4" s="43"/>
+      <c r="Z4" s="43"/>
+      <c r="AA4" s="43"/>
+      <c r="AB4" s="43"/>
+      <c r="AC4" s="43"/>
+      <c r="AD4" s="43"/>
+      <c r="AE4" s="43"/>
+      <c r="AF4" s="43"/>
+      <c r="AG4" s="43"/>
+      <c r="AH4" s="43"/>
+      <c r="AI4" s="43"/>
+      <c r="AJ4" s="43"/>
+      <c r="AK4" s="43"/>
+      <c r="AL4" s="43"/>
       <c r="AM4" s="6"/>
       <c r="AN4" s="6"/>
       <c r="AO4" s="6"/>
@@ -1679,17 +1687,17 @@
       <c r="AD5" s="10"/>
       <c r="AE5" s="10"/>
       <c r="AF5" s="10"/>
-      <c r="AG5" s="75" t="s">
+      <c r="AG5" s="44" t="s">
         <v>33</v>
       </c>
-      <c r="AH5" s="75"/>
-      <c r="AI5" s="75"/>
-      <c r="AJ5" s="75"/>
-      <c r="AK5" s="75"/>
-      <c r="AL5" s="75"/>
-      <c r="AM5" s="75"/>
-      <c r="AN5" s="75"/>
-      <c r="AO5" s="76"/>
+      <c r="AH5" s="44"/>
+      <c r="AI5" s="44"/>
+      <c r="AJ5" s="44"/>
+      <c r="AK5" s="44"/>
+      <c r="AL5" s="44"/>
+      <c r="AM5" s="44"/>
+      <c r="AN5" s="44"/>
+      <c r="AO5" s="45"/>
     </row>
     <row r="6" spans="1:41" ht="12.75">
       <c r="A6" s="6"/>
@@ -1759,11 +1767,11 @@
       <c r="T7" s="17"/>
       <c r="U7" s="17"/>
       <c r="V7" s="15"/>
-      <c r="W7" s="70" t="s">
+      <c r="W7" s="39" t="s">
         <v>35</v>
       </c>
-      <c r="X7" s="70"/>
-      <c r="Y7" s="70"/>
+      <c r="X7" s="39"/>
+      <c r="Y7" s="39"/>
       <c r="Z7" s="17"/>
       <c r="AA7" s="17"/>
       <c r="AB7" s="17"/>
@@ -1784,263 +1792,263 @@
     <row r="8" spans="1:41" ht="12.75">
       <c r="A8" s="6"/>
       <c r="B8" s="15"/>
-      <c r="C8" s="65" t="s">
+      <c r="C8" s="48" t="s">
         <v>36</v>
       </c>
-      <c r="D8" s="66"/>
-      <c r="E8" s="66"/>
-      <c r="F8" s="66"/>
-      <c r="G8" s="66"/>
-      <c r="H8" s="66"/>
-      <c r="I8" s="66"/>
-      <c r="J8" s="66"/>
-      <c r="K8" s="66"/>
-      <c r="L8" s="66"/>
-      <c r="M8" s="66"/>
-      <c r="N8" s="66"/>
-      <c r="O8" s="66"/>
-      <c r="P8" s="66"/>
-      <c r="Q8" s="66"/>
-      <c r="R8" s="66"/>
-      <c r="S8" s="66"/>
-      <c r="T8" s="66"/>
+      <c r="D8" s="49"/>
+      <c r="E8" s="49"/>
+      <c r="F8" s="49"/>
+      <c r="G8" s="49"/>
+      <c r="H8" s="49"/>
+      <c r="I8" s="49"/>
+      <c r="J8" s="49"/>
+      <c r="K8" s="49"/>
+      <c r="L8" s="49"/>
+      <c r="M8" s="49"/>
+      <c r="N8" s="49"/>
+      <c r="O8" s="49"/>
+      <c r="P8" s="49"/>
+      <c r="Q8" s="49"/>
+      <c r="R8" s="49"/>
+      <c r="S8" s="49"/>
+      <c r="T8" s="49"/>
       <c r="U8" s="17"/>
       <c r="V8" s="15"/>
-      <c r="W8" s="65" t="s">
+      <c r="W8" s="48" t="s">
         <v>37</v>
       </c>
-      <c r="X8" s="66"/>
-      <c r="Y8" s="66"/>
-      <c r="Z8" s="66"/>
-      <c r="AA8" s="66"/>
-      <c r="AB8" s="66"/>
-      <c r="AC8" s="66"/>
-      <c r="AD8" s="66"/>
-      <c r="AE8" s="66"/>
-      <c r="AF8" s="66"/>
-      <c r="AG8" s="66"/>
-      <c r="AH8" s="66"/>
-      <c r="AI8" s="66"/>
-      <c r="AJ8" s="66"/>
-      <c r="AK8" s="66"/>
-      <c r="AL8" s="66"/>
-      <c r="AM8" s="66"/>
-      <c r="AN8" s="66"/>
+      <c r="X8" s="49"/>
+      <c r="Y8" s="49"/>
+      <c r="Z8" s="49"/>
+      <c r="AA8" s="49"/>
+      <c r="AB8" s="49"/>
+      <c r="AC8" s="49"/>
+      <c r="AD8" s="49"/>
+      <c r="AE8" s="49"/>
+      <c r="AF8" s="49"/>
+      <c r="AG8" s="49"/>
+      <c r="AH8" s="49"/>
+      <c r="AI8" s="49"/>
+      <c r="AJ8" s="49"/>
+      <c r="AK8" s="49"/>
+      <c r="AL8" s="49"/>
+      <c r="AM8" s="49"/>
+      <c r="AN8" s="49"/>
       <c r="AO8" s="18"/>
     </row>
     <row r="9" spans="1:41" ht="12.75">
       <c r="A9" s="6"/>
       <c r="B9" s="15"/>
-      <c r="C9" s="66"/>
-      <c r="D9" s="66"/>
-      <c r="E9" s="66"/>
-      <c r="F9" s="66"/>
-      <c r="G9" s="66"/>
-      <c r="H9" s="66"/>
-      <c r="I9" s="66"/>
-      <c r="J9" s="66"/>
-      <c r="K9" s="66"/>
-      <c r="L9" s="66"/>
-      <c r="M9" s="66"/>
-      <c r="N9" s="66"/>
-      <c r="O9" s="66"/>
-      <c r="P9" s="66"/>
-      <c r="Q9" s="66"/>
-      <c r="R9" s="66"/>
-      <c r="S9" s="66"/>
-      <c r="T9" s="66"/>
+      <c r="C9" s="49"/>
+      <c r="D9" s="49"/>
+      <c r="E9" s="49"/>
+      <c r="F9" s="49"/>
+      <c r="G9" s="49"/>
+      <c r="H9" s="49"/>
+      <c r="I9" s="49"/>
+      <c r="J9" s="49"/>
+      <c r="K9" s="49"/>
+      <c r="L9" s="49"/>
+      <c r="M9" s="49"/>
+      <c r="N9" s="49"/>
+      <c r="O9" s="49"/>
+      <c r="P9" s="49"/>
+      <c r="Q9" s="49"/>
+      <c r="R9" s="49"/>
+      <c r="S9" s="49"/>
+      <c r="T9" s="49"/>
       <c r="U9" s="17"/>
       <c r="V9" s="15"/>
-      <c r="W9" s="66"/>
-      <c r="X9" s="66"/>
-      <c r="Y9" s="66"/>
-      <c r="Z9" s="66"/>
-      <c r="AA9" s="66"/>
-      <c r="AB9" s="66"/>
-      <c r="AC9" s="66"/>
-      <c r="AD9" s="66"/>
-      <c r="AE9" s="66"/>
-      <c r="AF9" s="66"/>
-      <c r="AG9" s="66"/>
-      <c r="AH9" s="66"/>
-      <c r="AI9" s="66"/>
-      <c r="AJ9" s="66"/>
-      <c r="AK9" s="66"/>
-      <c r="AL9" s="66"/>
-      <c r="AM9" s="66"/>
-      <c r="AN9" s="66"/>
+      <c r="W9" s="49"/>
+      <c r="X9" s="49"/>
+      <c r="Y9" s="49"/>
+      <c r="Z9" s="49"/>
+      <c r="AA9" s="49"/>
+      <c r="AB9" s="49"/>
+      <c r="AC9" s="49"/>
+      <c r="AD9" s="49"/>
+      <c r="AE9" s="49"/>
+      <c r="AF9" s="49"/>
+      <c r="AG9" s="49"/>
+      <c r="AH9" s="49"/>
+      <c r="AI9" s="49"/>
+      <c r="AJ9" s="49"/>
+      <c r="AK9" s="49"/>
+      <c r="AL9" s="49"/>
+      <c r="AM9" s="49"/>
+      <c r="AN9" s="49"/>
       <c r="AO9" s="18"/>
     </row>
     <row r="10" spans="1:41" ht="12.75">
       <c r="A10" s="6"/>
       <c r="B10" s="15"/>
-      <c r="C10" s="66"/>
-      <c r="D10" s="66"/>
-      <c r="E10" s="66"/>
-      <c r="F10" s="66"/>
-      <c r="G10" s="66"/>
-      <c r="H10" s="66"/>
-      <c r="I10" s="66"/>
-      <c r="J10" s="66"/>
-      <c r="K10" s="66"/>
-      <c r="L10" s="66"/>
-      <c r="M10" s="66"/>
-      <c r="N10" s="66"/>
-      <c r="O10" s="66"/>
-      <c r="P10" s="66"/>
-      <c r="Q10" s="66"/>
-      <c r="R10" s="66"/>
-      <c r="S10" s="66"/>
-      <c r="T10" s="66"/>
+      <c r="C10" s="49"/>
+      <c r="D10" s="49"/>
+      <c r="E10" s="49"/>
+      <c r="F10" s="49"/>
+      <c r="G10" s="49"/>
+      <c r="H10" s="49"/>
+      <c r="I10" s="49"/>
+      <c r="J10" s="49"/>
+      <c r="K10" s="49"/>
+      <c r="L10" s="49"/>
+      <c r="M10" s="49"/>
+      <c r="N10" s="49"/>
+      <c r="O10" s="49"/>
+      <c r="P10" s="49"/>
+      <c r="Q10" s="49"/>
+      <c r="R10" s="49"/>
+      <c r="S10" s="49"/>
+      <c r="T10" s="49"/>
       <c r="U10" s="17"/>
       <c r="V10" s="15"/>
-      <c r="W10" s="66"/>
-      <c r="X10" s="66"/>
-      <c r="Y10" s="66"/>
-      <c r="Z10" s="66"/>
-      <c r="AA10" s="66"/>
-      <c r="AB10" s="66"/>
-      <c r="AC10" s="66"/>
-      <c r="AD10" s="66"/>
-      <c r="AE10" s="66"/>
-      <c r="AF10" s="66"/>
-      <c r="AG10" s="66"/>
-      <c r="AH10" s="66"/>
-      <c r="AI10" s="66"/>
-      <c r="AJ10" s="66"/>
-      <c r="AK10" s="66"/>
-      <c r="AL10" s="66"/>
-      <c r="AM10" s="66"/>
-      <c r="AN10" s="66"/>
+      <c r="W10" s="49"/>
+      <c r="X10" s="49"/>
+      <c r="Y10" s="49"/>
+      <c r="Z10" s="49"/>
+      <c r="AA10" s="49"/>
+      <c r="AB10" s="49"/>
+      <c r="AC10" s="49"/>
+      <c r="AD10" s="49"/>
+      <c r="AE10" s="49"/>
+      <c r="AF10" s="49"/>
+      <c r="AG10" s="49"/>
+      <c r="AH10" s="49"/>
+      <c r="AI10" s="49"/>
+      <c r="AJ10" s="49"/>
+      <c r="AK10" s="49"/>
+      <c r="AL10" s="49"/>
+      <c r="AM10" s="49"/>
+      <c r="AN10" s="49"/>
       <c r="AO10" s="18"/>
     </row>
     <row r="11" spans="1:41" ht="12.75">
       <c r="A11" s="6"/>
       <c r="B11" s="15"/>
-      <c r="C11" s="66"/>
-      <c r="D11" s="66"/>
-      <c r="E11" s="66"/>
-      <c r="F11" s="66"/>
-      <c r="G11" s="66"/>
-      <c r="H11" s="66"/>
-      <c r="I11" s="66"/>
-      <c r="J11" s="66"/>
-      <c r="K11" s="66"/>
-      <c r="L11" s="66"/>
-      <c r="M11" s="66"/>
-      <c r="N11" s="66"/>
-      <c r="O11" s="66"/>
-      <c r="P11" s="66"/>
-      <c r="Q11" s="66"/>
-      <c r="R11" s="66"/>
-      <c r="S11" s="66"/>
-      <c r="T11" s="66"/>
+      <c r="C11" s="49"/>
+      <c r="D11" s="49"/>
+      <c r="E11" s="49"/>
+      <c r="F11" s="49"/>
+      <c r="G11" s="49"/>
+      <c r="H11" s="49"/>
+      <c r="I11" s="49"/>
+      <c r="J11" s="49"/>
+      <c r="K11" s="49"/>
+      <c r="L11" s="49"/>
+      <c r="M11" s="49"/>
+      <c r="N11" s="49"/>
+      <c r="O11" s="49"/>
+      <c r="P11" s="49"/>
+      <c r="Q11" s="49"/>
+      <c r="R11" s="49"/>
+      <c r="S11" s="49"/>
+      <c r="T11" s="49"/>
       <c r="U11" s="17"/>
       <c r="V11" s="15"/>
-      <c r="W11" s="66"/>
-      <c r="X11" s="66"/>
-      <c r="Y11" s="66"/>
-      <c r="Z11" s="66"/>
-      <c r="AA11" s="66"/>
-      <c r="AB11" s="66"/>
-      <c r="AC11" s="66"/>
-      <c r="AD11" s="66"/>
-      <c r="AE11" s="66"/>
-      <c r="AF11" s="66"/>
-      <c r="AG11" s="66"/>
-      <c r="AH11" s="66"/>
-      <c r="AI11" s="66"/>
-      <c r="AJ11" s="66"/>
-      <c r="AK11" s="66"/>
-      <c r="AL11" s="66"/>
-      <c r="AM11" s="66"/>
-      <c r="AN11" s="66"/>
+      <c r="W11" s="49"/>
+      <c r="X11" s="49"/>
+      <c r="Y11" s="49"/>
+      <c r="Z11" s="49"/>
+      <c r="AA11" s="49"/>
+      <c r="AB11" s="49"/>
+      <c r="AC11" s="49"/>
+      <c r="AD11" s="49"/>
+      <c r="AE11" s="49"/>
+      <c r="AF11" s="49"/>
+      <c r="AG11" s="49"/>
+      <c r="AH11" s="49"/>
+      <c r="AI11" s="49"/>
+      <c r="AJ11" s="49"/>
+      <c r="AK11" s="49"/>
+      <c r="AL11" s="49"/>
+      <c r="AM11" s="49"/>
+      <c r="AN11" s="49"/>
       <c r="AO11" s="18"/>
     </row>
     <row r="12" spans="1:41" ht="12.75">
       <c r="A12" s="6"/>
       <c r="B12" s="15"/>
-      <c r="C12" s="66"/>
-      <c r="D12" s="66"/>
-      <c r="E12" s="66"/>
-      <c r="F12" s="66"/>
-      <c r="G12" s="66"/>
-      <c r="H12" s="66"/>
-      <c r="I12" s="66"/>
-      <c r="J12" s="66"/>
-      <c r="K12" s="66"/>
-      <c r="L12" s="66"/>
-      <c r="M12" s="66"/>
-      <c r="N12" s="66"/>
-      <c r="O12" s="66"/>
-      <c r="P12" s="66"/>
-      <c r="Q12" s="66"/>
-      <c r="R12" s="66"/>
-      <c r="S12" s="66"/>
-      <c r="T12" s="66"/>
+      <c r="C12" s="49"/>
+      <c r="D12" s="49"/>
+      <c r="E12" s="49"/>
+      <c r="F12" s="49"/>
+      <c r="G12" s="49"/>
+      <c r="H12" s="49"/>
+      <c r="I12" s="49"/>
+      <c r="J12" s="49"/>
+      <c r="K12" s="49"/>
+      <c r="L12" s="49"/>
+      <c r="M12" s="49"/>
+      <c r="N12" s="49"/>
+      <c r="O12" s="49"/>
+      <c r="P12" s="49"/>
+      <c r="Q12" s="49"/>
+      <c r="R12" s="49"/>
+      <c r="S12" s="49"/>
+      <c r="T12" s="49"/>
       <c r="U12" s="17"/>
       <c r="V12" s="15"/>
-      <c r="W12" s="66"/>
-      <c r="X12" s="66"/>
-      <c r="Y12" s="66"/>
-      <c r="Z12" s="66"/>
-      <c r="AA12" s="66"/>
-      <c r="AB12" s="66"/>
-      <c r="AC12" s="66"/>
-      <c r="AD12" s="66"/>
-      <c r="AE12" s="66"/>
-      <c r="AF12" s="66"/>
-      <c r="AG12" s="66"/>
-      <c r="AH12" s="66"/>
-      <c r="AI12" s="66"/>
-      <c r="AJ12" s="66"/>
-      <c r="AK12" s="66"/>
-      <c r="AL12" s="66"/>
-      <c r="AM12" s="66"/>
-      <c r="AN12" s="66"/>
+      <c r="W12" s="49"/>
+      <c r="X12" s="49"/>
+      <c r="Y12" s="49"/>
+      <c r="Z12" s="49"/>
+      <c r="AA12" s="49"/>
+      <c r="AB12" s="49"/>
+      <c r="AC12" s="49"/>
+      <c r="AD12" s="49"/>
+      <c r="AE12" s="49"/>
+      <c r="AF12" s="49"/>
+      <c r="AG12" s="49"/>
+      <c r="AH12" s="49"/>
+      <c r="AI12" s="49"/>
+      <c r="AJ12" s="49"/>
+      <c r="AK12" s="49"/>
+      <c r="AL12" s="49"/>
+      <c r="AM12" s="49"/>
+      <c r="AN12" s="49"/>
       <c r="AO12" s="18"/>
     </row>
     <row r="13" spans="1:41" ht="12.75">
       <c r="A13" s="6"/>
       <c r="B13" s="15"/>
-      <c r="C13" s="66"/>
-      <c r="D13" s="66"/>
-      <c r="E13" s="66"/>
-      <c r="F13" s="66"/>
-      <c r="G13" s="66"/>
-      <c r="H13" s="66"/>
-      <c r="I13" s="66"/>
-      <c r="J13" s="66"/>
-      <c r="K13" s="66"/>
-      <c r="L13" s="66"/>
-      <c r="M13" s="66"/>
-      <c r="N13" s="66"/>
-      <c r="O13" s="66"/>
-      <c r="P13" s="66"/>
-      <c r="Q13" s="66"/>
-      <c r="R13" s="66"/>
-      <c r="S13" s="66"/>
-      <c r="T13" s="66"/>
+      <c r="C13" s="49"/>
+      <c r="D13" s="49"/>
+      <c r="E13" s="49"/>
+      <c r="F13" s="49"/>
+      <c r="G13" s="49"/>
+      <c r="H13" s="49"/>
+      <c r="I13" s="49"/>
+      <c r="J13" s="49"/>
+      <c r="K13" s="49"/>
+      <c r="L13" s="49"/>
+      <c r="M13" s="49"/>
+      <c r="N13" s="49"/>
+      <c r="O13" s="49"/>
+      <c r="P13" s="49"/>
+      <c r="Q13" s="49"/>
+      <c r="R13" s="49"/>
+      <c r="S13" s="49"/>
+      <c r="T13" s="49"/>
       <c r="U13" s="17"/>
       <c r="V13" s="15"/>
-      <c r="W13" s="66"/>
-      <c r="X13" s="66"/>
-      <c r="Y13" s="66"/>
-      <c r="Z13" s="66"/>
-      <c r="AA13" s="66"/>
-      <c r="AB13" s="66"/>
-      <c r="AC13" s="66"/>
-      <c r="AD13" s="66"/>
-      <c r="AE13" s="66"/>
-      <c r="AF13" s="66"/>
-      <c r="AG13" s="66"/>
-      <c r="AH13" s="66"/>
-      <c r="AI13" s="66"/>
-      <c r="AJ13" s="66"/>
-      <c r="AK13" s="66"/>
-      <c r="AL13" s="66"/>
-      <c r="AM13" s="66"/>
-      <c r="AN13" s="66"/>
+      <c r="W13" s="49"/>
+      <c r="X13" s="49"/>
+      <c r="Y13" s="49"/>
+      <c r="Z13" s="49"/>
+      <c r="AA13" s="49"/>
+      <c r="AB13" s="49"/>
+      <c r="AC13" s="49"/>
+      <c r="AD13" s="49"/>
+      <c r="AE13" s="49"/>
+      <c r="AF13" s="49"/>
+      <c r="AG13" s="49"/>
+      <c r="AH13" s="49"/>
+      <c r="AI13" s="49"/>
+      <c r="AJ13" s="49"/>
+      <c r="AK13" s="49"/>
+      <c r="AL13" s="49"/>
+      <c r="AM13" s="49"/>
+      <c r="AN13" s="49"/>
       <c r="AO13" s="18"/>
     </row>
     <row r="14" spans="1:41" ht="12.75">
@@ -2166,17 +2174,17 @@
       <c r="AB16" s="17" t="s">
         <v>40</v>
       </c>
-      <c r="AC16" s="67">
+      <c r="AC16" s="50">
         <v>47900266</v>
       </c>
-      <c r="AD16" s="67"/>
-      <c r="AE16" s="67"/>
-      <c r="AF16" s="67"/>
-      <c r="AG16" s="67"/>
-      <c r="AH16" s="67"/>
-      <c r="AI16" s="67"/>
-      <c r="AJ16" s="67"/>
-      <c r="AK16" s="67"/>
+      <c r="AD16" s="50"/>
+      <c r="AE16" s="50"/>
+      <c r="AF16" s="50"/>
+      <c r="AG16" s="50"/>
+      <c r="AH16" s="50"/>
+      <c r="AI16" s="50"/>
+      <c r="AJ16" s="50"/>
+      <c r="AK16" s="50"/>
       <c r="AL16" s="17"/>
       <c r="AM16" s="17"/>
       <c r="AN16" s="17"/>
@@ -2185,11 +2193,11 @@
     <row r="17" spans="1:41" ht="15">
       <c r="A17" s="6"/>
       <c r="B17" s="15"/>
-      <c r="C17" s="64" t="s">
+      <c r="C17" s="51" t="s">
         <v>41</v>
       </c>
-      <c r="D17" s="64"/>
-      <c r="E17" s="64"/>
+      <c r="D17" s="51"/>
+      <c r="E17" s="51"/>
       <c r="F17" s="23"/>
       <c r="G17" s="23"/>
       <c r="H17" s="23"/>
@@ -2217,17 +2225,17 @@
       <c r="AB17" s="17" t="s">
         <v>40</v>
       </c>
-      <c r="AC17" s="68">
+      <c r="AC17" s="52">
         <v>41865</v>
       </c>
-      <c r="AD17" s="68"/>
-      <c r="AE17" s="68"/>
-      <c r="AF17" s="68"/>
-      <c r="AG17" s="68"/>
-      <c r="AH17" s="68"/>
-      <c r="AI17" s="68"/>
-      <c r="AJ17" s="68"/>
-      <c r="AK17" s="68"/>
+      <c r="AD17" s="52"/>
+      <c r="AE17" s="52"/>
+      <c r="AF17" s="52"/>
+      <c r="AG17" s="52"/>
+      <c r="AH17" s="52"/>
+      <c r="AI17" s="52"/>
+      <c r="AJ17" s="52"/>
+      <c r="AK17" s="52"/>
       <c r="AL17" s="17"/>
       <c r="AM17" s="17"/>
       <c r="AN17" s="17"/>
@@ -2236,26 +2244,26 @@
     <row r="18" spans="1:41" ht="12.75">
       <c r="A18" s="6"/>
       <c r="B18" s="15"/>
-      <c r="C18" s="69" t="s">
+      <c r="C18" s="46" t="s">
         <v>43</v>
       </c>
-      <c r="D18" s="69"/>
-      <c r="E18" s="69"/>
-      <c r="F18" s="69"/>
-      <c r="G18" s="69"/>
-      <c r="H18" s="69"/>
-      <c r="I18" s="69"/>
-      <c r="J18" s="69"/>
-      <c r="K18" s="69"/>
-      <c r="L18" s="69"/>
-      <c r="M18" s="69"/>
-      <c r="N18" s="69"/>
-      <c r="O18" s="69"/>
-      <c r="P18" s="69"/>
-      <c r="Q18" s="69"/>
-      <c r="R18" s="69"/>
-      <c r="S18" s="69"/>
-      <c r="T18" s="69"/>
+      <c r="D18" s="46"/>
+      <c r="E18" s="46"/>
+      <c r="F18" s="46"/>
+      <c r="G18" s="46"/>
+      <c r="H18" s="46"/>
+      <c r="I18" s="46"/>
+      <c r="J18" s="46"/>
+      <c r="K18" s="46"/>
+      <c r="L18" s="46"/>
+      <c r="M18" s="46"/>
+      <c r="N18" s="46"/>
+      <c r="O18" s="46"/>
+      <c r="P18" s="46"/>
+      <c r="Q18" s="46"/>
+      <c r="R18" s="46"/>
+      <c r="S18" s="46"/>
+      <c r="T18" s="46"/>
       <c r="U18" s="18"/>
       <c r="V18" s="15"/>
       <c r="W18" s="17" t="s">
@@ -2268,17 +2276,17 @@
       <c r="AB18" s="17" t="s">
         <v>40</v>
       </c>
-      <c r="AC18" s="58" t="s">
+      <c r="AC18" s="47" t="s">
         <v>45</v>
       </c>
-      <c r="AD18" s="58"/>
-      <c r="AE18" s="58"/>
-      <c r="AF18" s="58"/>
-      <c r="AG18" s="58"/>
-      <c r="AH18" s="58"/>
-      <c r="AI18" s="58"/>
-      <c r="AJ18" s="58"/>
-      <c r="AK18" s="58"/>
+      <c r="AD18" s="47"/>
+      <c r="AE18" s="47"/>
+      <c r="AF18" s="47"/>
+      <c r="AG18" s="47"/>
+      <c r="AH18" s="47"/>
+      <c r="AI18" s="47"/>
+      <c r="AJ18" s="47"/>
+      <c r="AK18" s="47"/>
       <c r="AL18" s="17"/>
       <c r="AM18" s="17"/>
       <c r="AN18" s="17"/>
@@ -2287,24 +2295,24 @@
     <row r="19" spans="1:41" ht="12.75">
       <c r="A19" s="6"/>
       <c r="B19" s="15"/>
-      <c r="C19" s="69"/>
-      <c r="D19" s="69"/>
-      <c r="E19" s="69"/>
-      <c r="F19" s="69"/>
-      <c r="G19" s="69"/>
-      <c r="H19" s="69"/>
-      <c r="I19" s="69"/>
-      <c r="J19" s="69"/>
-      <c r="K19" s="69"/>
-      <c r="L19" s="69"/>
-      <c r="M19" s="69"/>
-      <c r="N19" s="69"/>
-      <c r="O19" s="69"/>
-      <c r="P19" s="69"/>
-      <c r="Q19" s="69"/>
-      <c r="R19" s="69"/>
-      <c r="S19" s="69"/>
-      <c r="T19" s="69"/>
+      <c r="C19" s="46"/>
+      <c r="D19" s="46"/>
+      <c r="E19" s="46"/>
+      <c r="F19" s="46"/>
+      <c r="G19" s="46"/>
+      <c r="H19" s="46"/>
+      <c r="I19" s="46"/>
+      <c r="J19" s="46"/>
+      <c r="K19" s="46"/>
+      <c r="L19" s="46"/>
+      <c r="M19" s="46"/>
+      <c r="N19" s="46"/>
+      <c r="O19" s="46"/>
+      <c r="P19" s="46"/>
+      <c r="Q19" s="46"/>
+      <c r="R19" s="46"/>
+      <c r="S19" s="46"/>
+      <c r="T19" s="46"/>
       <c r="U19" s="18"/>
       <c r="V19" s="15"/>
       <c r="W19" s="17" t="s">
@@ -2317,16 +2325,16 @@
       <c r="AB19" s="17" t="s">
         <v>40</v>
       </c>
-      <c r="AC19" s="58" t="s">
+      <c r="AC19" s="47" t="s">
         <v>47</v>
       </c>
-      <c r="AD19" s="58"/>
-      <c r="AE19" s="58"/>
-      <c r="AF19" s="58"/>
-      <c r="AG19" s="58"/>
-      <c r="AH19" s="58"/>
-      <c r="AI19" s="58"/>
-      <c r="AJ19" s="58"/>
+      <c r="AD19" s="47"/>
+      <c r="AE19" s="47"/>
+      <c r="AF19" s="47"/>
+      <c r="AG19" s="47"/>
+      <c r="AH19" s="47"/>
+      <c r="AI19" s="47"/>
+      <c r="AJ19" s="47"/>
       <c r="AK19" s="24"/>
       <c r="AL19" s="17"/>
       <c r="AM19" s="17"/>
@@ -2336,24 +2344,24 @@
     <row r="20" spans="1:41" ht="12.75">
       <c r="A20" s="6"/>
       <c r="B20" s="15"/>
-      <c r="C20" s="69"/>
-      <c r="D20" s="69"/>
-      <c r="E20" s="69"/>
-      <c r="F20" s="69"/>
-      <c r="G20" s="69"/>
-      <c r="H20" s="69"/>
-      <c r="I20" s="69"/>
-      <c r="J20" s="69"/>
-      <c r="K20" s="69"/>
-      <c r="L20" s="69"/>
-      <c r="M20" s="69"/>
-      <c r="N20" s="69"/>
-      <c r="O20" s="69"/>
-      <c r="P20" s="69"/>
-      <c r="Q20" s="69"/>
-      <c r="R20" s="69"/>
-      <c r="S20" s="69"/>
-      <c r="T20" s="69"/>
+      <c r="C20" s="46"/>
+      <c r="D20" s="46"/>
+      <c r="E20" s="46"/>
+      <c r="F20" s="46"/>
+      <c r="G20" s="46"/>
+      <c r="H20" s="46"/>
+      <c r="I20" s="46"/>
+      <c r="J20" s="46"/>
+      <c r="K20" s="46"/>
+      <c r="L20" s="46"/>
+      <c r="M20" s="46"/>
+      <c r="N20" s="46"/>
+      <c r="O20" s="46"/>
+      <c r="P20" s="46"/>
+      <c r="Q20" s="46"/>
+      <c r="R20" s="46"/>
+      <c r="S20" s="46"/>
+      <c r="T20" s="46"/>
       <c r="U20" s="18"/>
       <c r="V20" s="15"/>
       <c r="W20" s="17" t="s">
@@ -2366,17 +2374,17 @@
       <c r="AB20" s="17" t="s">
         <v>40</v>
       </c>
-      <c r="AC20" s="58" t="s">
+      <c r="AC20" s="47" t="s">
         <v>49</v>
       </c>
-      <c r="AD20" s="58"/>
-      <c r="AE20" s="58"/>
-      <c r="AF20" s="58"/>
-      <c r="AG20" s="58"/>
-      <c r="AH20" s="58"/>
-      <c r="AI20" s="58"/>
-      <c r="AJ20" s="58"/>
-      <c r="AK20" s="58"/>
+      <c r="AD20" s="47"/>
+      <c r="AE20" s="47"/>
+      <c r="AF20" s="47"/>
+      <c r="AG20" s="47"/>
+      <c r="AH20" s="47"/>
+      <c r="AI20" s="47"/>
+      <c r="AJ20" s="47"/>
+      <c r="AK20" s="47"/>
       <c r="AL20" s="17"/>
       <c r="AM20" s="17"/>
       <c r="AN20" s="17"/>
@@ -2385,24 +2393,24 @@
     <row r="21" spans="1:41" ht="12.75">
       <c r="A21" s="6"/>
       <c r="B21" s="15"/>
-      <c r="C21" s="69"/>
-      <c r="D21" s="69"/>
-      <c r="E21" s="69"/>
-      <c r="F21" s="69"/>
-      <c r="G21" s="69"/>
-      <c r="H21" s="69"/>
-      <c r="I21" s="69"/>
-      <c r="J21" s="69"/>
-      <c r="K21" s="69"/>
-      <c r="L21" s="69"/>
-      <c r="M21" s="69"/>
-      <c r="N21" s="69"/>
-      <c r="O21" s="69"/>
-      <c r="P21" s="69"/>
-      <c r="Q21" s="69"/>
-      <c r="R21" s="69"/>
-      <c r="S21" s="69"/>
-      <c r="T21" s="69"/>
+      <c r="C21" s="46"/>
+      <c r="D21" s="46"/>
+      <c r="E21" s="46"/>
+      <c r="F21" s="46"/>
+      <c r="G21" s="46"/>
+      <c r="H21" s="46"/>
+      <c r="I21" s="46"/>
+      <c r="J21" s="46"/>
+      <c r="K21" s="46"/>
+      <c r="L21" s="46"/>
+      <c r="M21" s="46"/>
+      <c r="N21" s="46"/>
+      <c r="O21" s="46"/>
+      <c r="P21" s="46"/>
+      <c r="Q21" s="46"/>
+      <c r="R21" s="46"/>
+      <c r="S21" s="46"/>
+      <c r="T21" s="46"/>
       <c r="U21" s="18"/>
       <c r="V21" s="15"/>
       <c r="W21" s="17"/>
@@ -2411,12 +2419,12 @@
       <c r="Z21" s="17"/>
       <c r="AA21" s="17"/>
       <c r="AB21" s="17"/>
-      <c r="AC21" s="58"/>
-      <c r="AD21" s="58"/>
-      <c r="AE21" s="58"/>
-      <c r="AF21" s="58"/>
-      <c r="AG21" s="58"/>
-      <c r="AH21" s="58"/>
+      <c r="AC21" s="47"/>
+      <c r="AD21" s="47"/>
+      <c r="AE21" s="47"/>
+      <c r="AF21" s="47"/>
+      <c r="AG21" s="47"/>
+      <c r="AH21" s="47"/>
       <c r="AI21" s="17"/>
       <c r="AJ21" s="17"/>
       <c r="AK21" s="17"/>
@@ -2428,24 +2436,24 @@
     <row r="22" spans="1:41" ht="15">
       <c r="A22" s="6"/>
       <c r="B22" s="15"/>
-      <c r="C22" s="64"/>
-      <c r="D22" s="64"/>
-      <c r="E22" s="64"/>
-      <c r="F22" s="64"/>
-      <c r="G22" s="64"/>
-      <c r="H22" s="64"/>
-      <c r="I22" s="64"/>
-      <c r="J22" s="64"/>
-      <c r="K22" s="64"/>
-      <c r="L22" s="64"/>
-      <c r="M22" s="64"/>
-      <c r="N22" s="64"/>
-      <c r="O22" s="64"/>
-      <c r="P22" s="64"/>
-      <c r="Q22" s="64"/>
-      <c r="R22" s="64"/>
-      <c r="S22" s="64"/>
-      <c r="T22" s="64"/>
+      <c r="C22" s="51"/>
+      <c r="D22" s="51"/>
+      <c r="E22" s="51"/>
+      <c r="F22" s="51"/>
+      <c r="G22" s="51"/>
+      <c r="H22" s="51"/>
+      <c r="I22" s="51"/>
+      <c r="J22" s="51"/>
+      <c r="K22" s="51"/>
+      <c r="L22" s="51"/>
+      <c r="M22" s="51"/>
+      <c r="N22" s="51"/>
+      <c r="O22" s="51"/>
+      <c r="P22" s="51"/>
+      <c r="Q22" s="51"/>
+      <c r="R22" s="51"/>
+      <c r="S22" s="51"/>
+      <c r="T22" s="51"/>
       <c r="U22" s="18"/>
       <c r="V22" s="15"/>
       <c r="W22" s="17"/>
@@ -2454,12 +2462,12 @@
       <c r="Z22" s="17"/>
       <c r="AA22" s="17"/>
       <c r="AB22" s="17"/>
-      <c r="AC22" s="58"/>
-      <c r="AD22" s="58"/>
-      <c r="AE22" s="58"/>
-      <c r="AF22" s="58"/>
-      <c r="AG22" s="58"/>
-      <c r="AH22" s="58"/>
+      <c r="AC22" s="47"/>
+      <c r="AD22" s="47"/>
+      <c r="AE22" s="47"/>
+      <c r="AF22" s="47"/>
+      <c r="AG22" s="47"/>
+      <c r="AH22" s="47"/>
       <c r="AI22" s="17"/>
       <c r="AJ22" s="17"/>
       <c r="AK22" s="17"/>
@@ -2549,115 +2557,115 @@
       <c r="AI24" s="13"/>
       <c r="AJ24" s="13"/>
       <c r="AK24" s="13"/>
-      <c r="AL24" s="59" t="s">
+      <c r="AL24" s="53" t="s">
         <v>50</v>
       </c>
-      <c r="AM24" s="59"/>
-      <c r="AN24" s="59"/>
+      <c r="AM24" s="53"/>
+      <c r="AN24" s="53"/>
       <c r="AO24" s="14"/>
     </row>
     <row r="25" spans="1:41" ht="12.75">
       <c r="A25" s="6"/>
       <c r="B25" s="15"/>
-      <c r="C25" s="60" t="s">
+      <c r="C25" s="54" t="s">
         <v>51</v>
       </c>
-      <c r="D25" s="60"/>
-      <c r="E25" s="60"/>
-      <c r="F25" s="60"/>
+      <c r="D25" s="54"/>
+      <c r="E25" s="54"/>
+      <c r="F25" s="54"/>
       <c r="G25" s="25"/>
-      <c r="H25" s="61" t="s">
+      <c r="H25" s="55" t="s">
         <v>52</v>
       </c>
-      <c r="I25" s="61"/>
-      <c r="J25" s="61"/>
+      <c r="I25" s="55"/>
+      <c r="J25" s="55"/>
       <c r="K25" s="25"/>
-      <c r="L25" s="62" t="s">
+      <c r="L25" s="56" t="s">
         <v>53</v>
       </c>
-      <c r="M25" s="62"/>
-      <c r="N25" s="62"/>
-      <c r="O25" s="62"/>
-      <c r="P25" s="62"/>
+      <c r="M25" s="56"/>
+      <c r="N25" s="56"/>
+      <c r="O25" s="56"/>
+      <c r="P25" s="56"/>
       <c r="Q25" s="26"/>
-      <c r="R25" s="63" t="s">
+      <c r="R25" s="57" t="s">
         <v>54</v>
       </c>
-      <c r="S25" s="63"/>
-      <c r="T25" s="63"/>
-      <c r="U25" s="63"/>
-      <c r="V25" s="63"/>
-      <c r="W25" s="63"/>
-      <c r="X25" s="63"/>
-      <c r="Y25" s="63"/>
-      <c r="Z25" s="63"/>
-      <c r="AA25" s="63"/>
-      <c r="AB25" s="63"/>
-      <c r="AC25" s="63"/>
-      <c r="AD25" s="63"/>
-      <c r="AE25" s="63" t="s">
+      <c r="S25" s="57"/>
+      <c r="T25" s="57"/>
+      <c r="U25" s="57"/>
+      <c r="V25" s="57"/>
+      <c r="W25" s="57"/>
+      <c r="X25" s="57"/>
+      <c r="Y25" s="57"/>
+      <c r="Z25" s="57"/>
+      <c r="AA25" s="57"/>
+      <c r="AB25" s="57"/>
+      <c r="AC25" s="57"/>
+      <c r="AD25" s="57"/>
+      <c r="AE25" s="57" t="s">
         <v>55</v>
       </c>
-      <c r="AF25" s="63"/>
+      <c r="AF25" s="57"/>
       <c r="AG25" s="25"/>
-      <c r="AH25" s="60" t="str">
+      <c r="AH25" s="54" t="str">
         <f>CONCATENATE("UNIT PRICE",CHAR(10),"(",AL24,")")</f>
         <v>UNIT PRICE
 (SGD)</v>
       </c>
-      <c r="AI25" s="60"/>
-      <c r="AJ25" s="60"/>
+      <c r="AI25" s="54"/>
+      <c r="AJ25" s="54"/>
       <c r="AK25" s="25"/>
-      <c r="AL25" s="60" t="str">
+      <c r="AL25" s="54" t="str">
         <f>CONCATENATE("TOTAL",CHAR(10),"(",AL24,")")</f>
         <v>TOTAL
 (SGD)</v>
       </c>
-      <c r="AM25" s="60"/>
-      <c r="AN25" s="60"/>
+      <c r="AM25" s="54"/>
+      <c r="AN25" s="54"/>
       <c r="AO25" s="18"/>
     </row>
     <row r="26" spans="1:41" ht="12.75">
       <c r="A26" s="6"/>
       <c r="B26" s="15"/>
-      <c r="C26" s="60"/>
-      <c r="D26" s="60"/>
-      <c r="E26" s="60"/>
-      <c r="F26" s="60"/>
+      <c r="C26" s="54"/>
+      <c r="D26" s="54"/>
+      <c r="E26" s="54"/>
+      <c r="F26" s="54"/>
       <c r="G26" s="25"/>
-      <c r="H26" s="61"/>
-      <c r="I26" s="61"/>
-      <c r="J26" s="61"/>
+      <c r="H26" s="55"/>
+      <c r="I26" s="55"/>
+      <c r="J26" s="55"/>
       <c r="K26" s="25"/>
-      <c r="L26" s="62"/>
-      <c r="M26" s="62"/>
-      <c r="N26" s="62"/>
-      <c r="O26" s="62"/>
-      <c r="P26" s="62"/>
+      <c r="L26" s="56"/>
+      <c r="M26" s="56"/>
+      <c r="N26" s="56"/>
+      <c r="O26" s="56"/>
+      <c r="P26" s="56"/>
       <c r="Q26" s="26"/>
-      <c r="R26" s="63"/>
-      <c r="S26" s="63"/>
-      <c r="T26" s="63"/>
-      <c r="U26" s="63"/>
-      <c r="V26" s="63"/>
-      <c r="W26" s="63"/>
-      <c r="X26" s="63"/>
-      <c r="Y26" s="63"/>
-      <c r="Z26" s="63"/>
-      <c r="AA26" s="63"/>
-      <c r="AB26" s="63"/>
-      <c r="AC26" s="63"/>
-      <c r="AD26" s="63"/>
-      <c r="AE26" s="63"/>
-      <c r="AF26" s="63"/>
+      <c r="R26" s="57"/>
+      <c r="S26" s="57"/>
+      <c r="T26" s="57"/>
+      <c r="U26" s="57"/>
+      <c r="V26" s="57"/>
+      <c r="W26" s="57"/>
+      <c r="X26" s="57"/>
+      <c r="Y26" s="57"/>
+      <c r="Z26" s="57"/>
+      <c r="AA26" s="57"/>
+      <c r="AB26" s="57"/>
+      <c r="AC26" s="57"/>
+      <c r="AD26" s="57"/>
+      <c r="AE26" s="57"/>
+      <c r="AF26" s="57"/>
       <c r="AG26" s="25"/>
-      <c r="AH26" s="60"/>
-      <c r="AI26" s="60"/>
-      <c r="AJ26" s="60"/>
+      <c r="AH26" s="54"/>
+      <c r="AI26" s="54"/>
+      <c r="AJ26" s="54"/>
       <c r="AK26" s="25"/>
-      <c r="AL26" s="60"/>
-      <c r="AM26" s="60"/>
-      <c r="AN26" s="60"/>
+      <c r="AL26" s="54"/>
+      <c r="AM26" s="54"/>
+      <c r="AN26" s="54"/>
       <c r="AO26" s="18"/>
     </row>
     <row r="27" spans="1:41" ht="12.75">
@@ -2705,381 +2713,381 @@
     </row>
     <row r="28" spans="1:41" ht="12.75">
       <c r="A28" s="6"/>
-      <c r="B28" s="55"/>
-      <c r="C28" s="56"/>
-      <c r="D28" s="56"/>
-      <c r="E28" s="56"/>
-      <c r="F28" s="56"/>
-      <c r="G28" s="56"/>
-      <c r="H28" s="56"/>
-      <c r="I28" s="56"/>
-      <c r="J28" s="56"/>
-      <c r="K28" s="56"/>
-      <c r="L28" s="56"/>
-      <c r="M28" s="56"/>
-      <c r="N28" s="56"/>
-      <c r="O28" s="56"/>
-      <c r="P28" s="56"/>
-      <c r="Q28" s="56"/>
-      <c r="R28" s="56"/>
-      <c r="S28" s="56"/>
-      <c r="T28" s="56"/>
-      <c r="U28" s="56"/>
-      <c r="V28" s="56"/>
-      <c r="W28" s="56"/>
-      <c r="X28" s="56"/>
-      <c r="Y28" s="56"/>
-      <c r="Z28" s="56"/>
-      <c r="AA28" s="56"/>
-      <c r="AB28" s="56"/>
-      <c r="AC28" s="56"/>
-      <c r="AD28" s="56"/>
-      <c r="AE28" s="56"/>
-      <c r="AF28" s="56"/>
-      <c r="AG28" s="56"/>
-      <c r="AH28" s="56"/>
-      <c r="AI28" s="56"/>
-      <c r="AJ28" s="56"/>
-      <c r="AK28" s="56"/>
-      <c r="AL28" s="56"/>
-      <c r="AM28" s="56"/>
-      <c r="AN28" s="56"/>
-      <c r="AO28" s="57"/>
+      <c r="B28" s="58"/>
+      <c r="C28" s="59"/>
+      <c r="D28" s="59"/>
+      <c r="E28" s="59"/>
+      <c r="F28" s="59"/>
+      <c r="G28" s="59"/>
+      <c r="H28" s="59"/>
+      <c r="I28" s="59"/>
+      <c r="J28" s="59"/>
+      <c r="K28" s="59"/>
+      <c r="L28" s="59"/>
+      <c r="M28" s="59"/>
+      <c r="N28" s="59"/>
+      <c r="O28" s="59"/>
+      <c r="P28" s="59"/>
+      <c r="Q28" s="59"/>
+      <c r="R28" s="59"/>
+      <c r="S28" s="59"/>
+      <c r="T28" s="59"/>
+      <c r="U28" s="59"/>
+      <c r="V28" s="59"/>
+      <c r="W28" s="59"/>
+      <c r="X28" s="59"/>
+      <c r="Y28" s="59"/>
+      <c r="Z28" s="59"/>
+      <c r="AA28" s="59"/>
+      <c r="AB28" s="59"/>
+      <c r="AC28" s="59"/>
+      <c r="AD28" s="59"/>
+      <c r="AE28" s="59"/>
+      <c r="AF28" s="59"/>
+      <c r="AG28" s="59"/>
+      <c r="AH28" s="59"/>
+      <c r="AI28" s="59"/>
+      <c r="AJ28" s="59"/>
+      <c r="AK28" s="59"/>
+      <c r="AL28" s="59"/>
+      <c r="AM28" s="59"/>
+      <c r="AN28" s="59"/>
+      <c r="AO28" s="60"/>
     </row>
     <row r="29" spans="1:41" s="11" customFormat="1" ht="87.75" customHeight="1">
       <c r="A29" s="8"/>
       <c r="B29" s="28"/>
-      <c r="C29" s="49">
+      <c r="C29" s="61">
         <v>41955</v>
       </c>
-      <c r="D29" s="49"/>
-      <c r="E29" s="49"/>
-      <c r="F29" s="49"/>
+      <c r="D29" s="61"/>
+      <c r="E29" s="61"/>
+      <c r="F29" s="61"/>
       <c r="G29" s="29"/>
-      <c r="H29" s="50" t="s">
+      <c r="H29" s="62" t="s">
         <v>56</v>
       </c>
-      <c r="I29" s="51"/>
-      <c r="J29" s="51"/>
+      <c r="I29" s="63"/>
+      <c r="J29" s="63"/>
       <c r="K29" s="29"/>
-      <c r="L29" s="54" t="s">
+      <c r="L29" s="68" t="s">
         <v>57</v>
       </c>
-      <c r="M29" s="54"/>
-      <c r="N29" s="54"/>
-      <c r="O29" s="54"/>
-      <c r="P29" s="54"/>
+      <c r="M29" s="68"/>
+      <c r="N29" s="68"/>
+      <c r="O29" s="68"/>
+      <c r="P29" s="68"/>
       <c r="Q29" s="30"/>
-      <c r="R29" s="52" t="s">
+      <c r="R29" s="64" t="s">
         <v>58</v>
       </c>
-      <c r="S29" s="52"/>
-      <c r="T29" s="52"/>
-      <c r="U29" s="52"/>
-      <c r="V29" s="52"/>
-      <c r="W29" s="52"/>
-      <c r="X29" s="52"/>
-      <c r="Y29" s="52"/>
-      <c r="Z29" s="52"/>
-      <c r="AA29" s="52"/>
-      <c r="AB29" s="52"/>
-      <c r="AC29" s="52"/>
-      <c r="AD29" s="52"/>
-      <c r="AE29" s="51">
+      <c r="S29" s="64"/>
+      <c r="T29" s="64"/>
+      <c r="U29" s="64"/>
+      <c r="V29" s="64"/>
+      <c r="W29" s="64"/>
+      <c r="X29" s="64"/>
+      <c r="Y29" s="64"/>
+      <c r="Z29" s="64"/>
+      <c r="AA29" s="64"/>
+      <c r="AB29" s="64"/>
+      <c r="AC29" s="64"/>
+      <c r="AD29" s="64"/>
+      <c r="AE29" s="63">
         <v>30</v>
       </c>
-      <c r="AF29" s="51"/>
+      <c r="AF29" s="63"/>
       <c r="AG29" s="29"/>
-      <c r="AH29" s="53">
+      <c r="AH29" s="65">
         <v>900</v>
       </c>
-      <c r="AI29" s="53"/>
-      <c r="AJ29" s="53"/>
+      <c r="AI29" s="65"/>
+      <c r="AJ29" s="65"/>
       <c r="AK29" s="29"/>
-      <c r="AL29" s="47">
+      <c r="AL29" s="66">
         <f>AE29*AH29</f>
         <v>27000</v>
       </c>
-      <c r="AM29" s="47"/>
-      <c r="AN29" s="47"/>
-      <c r="AO29" s="48"/>
+      <c r="AM29" s="66"/>
+      <c r="AN29" s="66"/>
+      <c r="AO29" s="67"/>
     </row>
     <row r="30" spans="1:41" s="11" customFormat="1" ht="87.75" customHeight="1">
       <c r="A30" s="8"/>
       <c r="B30" s="28"/>
-      <c r="C30" s="49">
+      <c r="C30" s="61">
         <v>41955</v>
       </c>
-      <c r="D30" s="49"/>
-      <c r="E30" s="49"/>
-      <c r="F30" s="49"/>
+      <c r="D30" s="61"/>
+      <c r="E30" s="61"/>
+      <c r="F30" s="61"/>
       <c r="G30" s="29"/>
-      <c r="H30" s="50" t="s">
+      <c r="H30" s="62" t="s">
         <v>59</v>
       </c>
-      <c r="I30" s="51"/>
-      <c r="J30" s="51"/>
+      <c r="I30" s="63"/>
+      <c r="J30" s="63"/>
       <c r="K30" s="29"/>
-      <c r="L30" s="54" t="s">
+      <c r="L30" s="68" t="s">
         <v>57</v>
       </c>
-      <c r="M30" s="54"/>
-      <c r="N30" s="54"/>
-      <c r="O30" s="54"/>
-      <c r="P30" s="54"/>
+      <c r="M30" s="68"/>
+      <c r="N30" s="68"/>
+      <c r="O30" s="68"/>
+      <c r="P30" s="68"/>
       <c r="Q30" s="30"/>
-      <c r="R30" s="52" t="s">
+      <c r="R30" s="64" t="s">
         <v>58</v>
       </c>
-      <c r="S30" s="52"/>
-      <c r="T30" s="52"/>
-      <c r="U30" s="52"/>
-      <c r="V30" s="52"/>
-      <c r="W30" s="52"/>
-      <c r="X30" s="52"/>
-      <c r="Y30" s="52"/>
-      <c r="Z30" s="52"/>
-      <c r="AA30" s="52"/>
-      <c r="AB30" s="52"/>
-      <c r="AC30" s="52"/>
-      <c r="AD30" s="52"/>
-      <c r="AE30" s="51">
+      <c r="S30" s="64"/>
+      <c r="T30" s="64"/>
+      <c r="U30" s="64"/>
+      <c r="V30" s="64"/>
+      <c r="W30" s="64"/>
+      <c r="X30" s="64"/>
+      <c r="Y30" s="64"/>
+      <c r="Z30" s="64"/>
+      <c r="AA30" s="64"/>
+      <c r="AB30" s="64"/>
+      <c r="AC30" s="64"/>
+      <c r="AD30" s="64"/>
+      <c r="AE30" s="63">
         <v>30</v>
       </c>
-      <c r="AF30" s="51"/>
+      <c r="AF30" s="63"/>
       <c r="AG30" s="29"/>
-      <c r="AH30" s="53">
+      <c r="AH30" s="65">
         <v>900</v>
       </c>
-      <c r="AI30" s="53"/>
-      <c r="AJ30" s="53"/>
+      <c r="AI30" s="65"/>
+      <c r="AJ30" s="65"/>
       <c r="AK30" s="29"/>
-      <c r="AL30" s="47">
+      <c r="AL30" s="66">
         <f>AE30*AH30</f>
         <v>27000</v>
       </c>
-      <c r="AM30" s="47"/>
-      <c r="AN30" s="47"/>
-      <c r="AO30" s="48"/>
+      <c r="AM30" s="66"/>
+      <c r="AN30" s="66"/>
+      <c r="AO30" s="67"/>
     </row>
     <row r="31" spans="1:41" s="11" customFormat="1" ht="87.75" customHeight="1">
       <c r="A31" s="8"/>
       <c r="B31" s="28"/>
-      <c r="C31" s="49">
+      <c r="C31" s="61">
         <v>41955</v>
       </c>
-      <c r="D31" s="49"/>
-      <c r="E31" s="49"/>
-      <c r="F31" s="49"/>
+      <c r="D31" s="61"/>
+      <c r="E31" s="61"/>
+      <c r="F31" s="61"/>
       <c r="G31" s="29"/>
-      <c r="H31" s="50" t="s">
+      <c r="H31" s="62" t="s">
         <v>60</v>
       </c>
-      <c r="I31" s="51"/>
-      <c r="J31" s="51"/>
+      <c r="I31" s="63"/>
+      <c r="J31" s="63"/>
       <c r="K31" s="29"/>
-      <c r="L31" s="54" t="s">
+      <c r="L31" s="68" t="s">
         <v>57</v>
       </c>
-      <c r="M31" s="54"/>
-      <c r="N31" s="54"/>
-      <c r="O31" s="54"/>
-      <c r="P31" s="54"/>
+      <c r="M31" s="68"/>
+      <c r="N31" s="68"/>
+      <c r="O31" s="68"/>
+      <c r="P31" s="68"/>
       <c r="Q31" s="30"/>
-      <c r="R31" s="52" t="s">
+      <c r="R31" s="64" t="s">
         <v>58</v>
       </c>
-      <c r="S31" s="52"/>
-      <c r="T31" s="52"/>
-      <c r="U31" s="52"/>
-      <c r="V31" s="52"/>
-      <c r="W31" s="52"/>
-      <c r="X31" s="52"/>
-      <c r="Y31" s="52"/>
-      <c r="Z31" s="52"/>
-      <c r="AA31" s="52"/>
-      <c r="AB31" s="52"/>
-      <c r="AC31" s="52"/>
-      <c r="AD31" s="52"/>
-      <c r="AE31" s="51">
+      <c r="S31" s="64"/>
+      <c r="T31" s="64"/>
+      <c r="U31" s="64"/>
+      <c r="V31" s="64"/>
+      <c r="W31" s="64"/>
+      <c r="X31" s="64"/>
+      <c r="Y31" s="64"/>
+      <c r="Z31" s="64"/>
+      <c r="AA31" s="64"/>
+      <c r="AB31" s="64"/>
+      <c r="AC31" s="64"/>
+      <c r="AD31" s="64"/>
+      <c r="AE31" s="63">
         <v>30</v>
       </c>
-      <c r="AF31" s="51"/>
+      <c r="AF31" s="63"/>
       <c r="AG31" s="29"/>
-      <c r="AH31" s="53">
+      <c r="AH31" s="65">
         <v>900</v>
       </c>
-      <c r="AI31" s="53"/>
-      <c r="AJ31" s="53"/>
+      <c r="AI31" s="65"/>
+      <c r="AJ31" s="65"/>
       <c r="AK31" s="29"/>
-      <c r="AL31" s="47">
+      <c r="AL31" s="66">
         <f>AE31*AH31</f>
         <v>27000</v>
       </c>
-      <c r="AM31" s="47"/>
-      <c r="AN31" s="47"/>
-      <c r="AO31" s="48"/>
+      <c r="AM31" s="66"/>
+      <c r="AN31" s="66"/>
+      <c r="AO31" s="67"/>
     </row>
     <row r="32" spans="1:41" s="11" customFormat="1" ht="87.75" customHeight="1">
       <c r="A32" s="8"/>
       <c r="B32" s="28"/>
-      <c r="C32" s="49">
+      <c r="C32" s="61">
         <v>41955</v>
       </c>
-      <c r="D32" s="49"/>
-      <c r="E32" s="49"/>
-      <c r="F32" s="49"/>
+      <c r="D32" s="61"/>
+      <c r="E32" s="61"/>
+      <c r="F32" s="61"/>
       <c r="G32" s="29"/>
-      <c r="H32" s="50" t="s">
+      <c r="H32" s="62" t="s">
         <v>61</v>
       </c>
-      <c r="I32" s="51"/>
-      <c r="J32" s="51"/>
+      <c r="I32" s="63"/>
+      <c r="J32" s="63"/>
       <c r="K32" s="29"/>
-      <c r="L32" s="54" t="s">
+      <c r="L32" s="68" t="s">
         <v>57</v>
       </c>
-      <c r="M32" s="54"/>
-      <c r="N32" s="54"/>
-      <c r="O32" s="54"/>
-      <c r="P32" s="54"/>
+      <c r="M32" s="68"/>
+      <c r="N32" s="68"/>
+      <c r="O32" s="68"/>
+      <c r="P32" s="68"/>
       <c r="Q32" s="30"/>
-      <c r="R32" s="52" t="s">
+      <c r="R32" s="64" t="s">
         <v>58</v>
       </c>
-      <c r="S32" s="52"/>
-      <c r="T32" s="52"/>
-      <c r="U32" s="52"/>
-      <c r="V32" s="52"/>
-      <c r="W32" s="52"/>
-      <c r="X32" s="52"/>
-      <c r="Y32" s="52"/>
-      <c r="Z32" s="52"/>
-      <c r="AA32" s="52"/>
-      <c r="AB32" s="52"/>
-      <c r="AC32" s="52"/>
-      <c r="AD32" s="52"/>
-      <c r="AE32" s="51">
+      <c r="S32" s="64"/>
+      <c r="T32" s="64"/>
+      <c r="U32" s="64"/>
+      <c r="V32" s="64"/>
+      <c r="W32" s="64"/>
+      <c r="X32" s="64"/>
+      <c r="Y32" s="64"/>
+      <c r="Z32" s="64"/>
+      <c r="AA32" s="64"/>
+      <c r="AB32" s="64"/>
+      <c r="AC32" s="64"/>
+      <c r="AD32" s="64"/>
+      <c r="AE32" s="63">
         <v>30</v>
       </c>
-      <c r="AF32" s="51"/>
+      <c r="AF32" s="63"/>
       <c r="AG32" s="29"/>
-      <c r="AH32" s="53">
+      <c r="AH32" s="65">
         <v>900</v>
       </c>
-      <c r="AI32" s="53"/>
-      <c r="AJ32" s="53"/>
+      <c r="AI32" s="65"/>
+      <c r="AJ32" s="65"/>
       <c r="AK32" s="29"/>
-      <c r="AL32" s="47">
+      <c r="AL32" s="66">
         <f>AE32*AH32</f>
         <v>27000</v>
       </c>
-      <c r="AM32" s="47"/>
-      <c r="AN32" s="47"/>
-      <c r="AO32" s="48"/>
+      <c r="AM32" s="66"/>
+      <c r="AN32" s="66"/>
+      <c r="AO32" s="67"/>
     </row>
     <row r="33" spans="1:41" s="11" customFormat="1" ht="87.75" customHeight="1">
       <c r="A33" s="8"/>
       <c r="B33" s="28"/>
-      <c r="C33" s="49">
+      <c r="C33" s="61">
         <v>41955</v>
       </c>
-      <c r="D33" s="49"/>
-      <c r="E33" s="49"/>
-      <c r="F33" s="49"/>
+      <c r="D33" s="61"/>
+      <c r="E33" s="61"/>
+      <c r="F33" s="61"/>
       <c r="G33" s="29"/>
-      <c r="H33" s="50" t="s">
+      <c r="H33" s="62" t="s">
         <v>62</v>
       </c>
-      <c r="I33" s="51"/>
-      <c r="J33" s="51"/>
+      <c r="I33" s="63"/>
+      <c r="J33" s="63"/>
       <c r="K33" s="29"/>
-      <c r="L33" s="54" t="s">
+      <c r="L33" s="68" t="s">
         <v>57</v>
       </c>
-      <c r="M33" s="54"/>
-      <c r="N33" s="54"/>
-      <c r="O33" s="54"/>
-      <c r="P33" s="54"/>
+      <c r="M33" s="68"/>
+      <c r="N33" s="68"/>
+      <c r="O33" s="68"/>
+      <c r="P33" s="68"/>
       <c r="Q33" s="30"/>
-      <c r="R33" s="52" t="s">
+      <c r="R33" s="64" t="s">
         <v>58</v>
       </c>
-      <c r="S33" s="52"/>
-      <c r="T33" s="52"/>
-      <c r="U33" s="52"/>
-      <c r="V33" s="52"/>
-      <c r="W33" s="52"/>
-      <c r="X33" s="52"/>
-      <c r="Y33" s="52"/>
-      <c r="Z33" s="52"/>
-      <c r="AA33" s="52"/>
-      <c r="AB33" s="52"/>
-      <c r="AC33" s="52"/>
-      <c r="AD33" s="52"/>
-      <c r="AE33" s="51">
+      <c r="S33" s="64"/>
+      <c r="T33" s="64"/>
+      <c r="U33" s="64"/>
+      <c r="V33" s="64"/>
+      <c r="W33" s="64"/>
+      <c r="X33" s="64"/>
+      <c r="Y33" s="64"/>
+      <c r="Z33" s="64"/>
+      <c r="AA33" s="64"/>
+      <c r="AB33" s="64"/>
+      <c r="AC33" s="64"/>
+      <c r="AD33" s="64"/>
+      <c r="AE33" s="63">
         <v>30</v>
       </c>
-      <c r="AF33" s="51"/>
+      <c r="AF33" s="63"/>
       <c r="AG33" s="29"/>
-      <c r="AH33" s="53">
+      <c r="AH33" s="65">
         <v>900</v>
       </c>
-      <c r="AI33" s="53"/>
-      <c r="AJ33" s="53"/>
+      <c r="AI33" s="65"/>
+      <c r="AJ33" s="65"/>
       <c r="AK33" s="29"/>
-      <c r="AL33" s="47">
+      <c r="AL33" s="66">
         <f>AE33*AH33</f>
         <v>27000</v>
       </c>
-      <c r="AM33" s="47"/>
-      <c r="AN33" s="47"/>
-      <c r="AO33" s="48"/>
+      <c r="AM33" s="66"/>
+      <c r="AN33" s="66"/>
+      <c r="AO33" s="67"/>
     </row>
     <row r="34" spans="1:41" ht="12.75">
       <c r="A34" s="6"/>
-      <c r="B34" s="39" t="s">
+      <c r="B34" s="69" t="s">
         <v>63</v>
       </c>
-      <c r="C34" s="40"/>
-      <c r="D34" s="40"/>
-      <c r="E34" s="40"/>
-      <c r="F34" s="40"/>
-      <c r="G34" s="40"/>
-      <c r="H34" s="40"/>
-      <c r="I34" s="40"/>
-      <c r="J34" s="40"/>
-      <c r="K34" s="40"/>
-      <c r="L34" s="40"/>
-      <c r="M34" s="40"/>
-      <c r="N34" s="40"/>
-      <c r="O34" s="40"/>
-      <c r="P34" s="40"/>
-      <c r="Q34" s="40"/>
-      <c r="R34" s="40"/>
-      <c r="S34" s="40"/>
-      <c r="T34" s="40"/>
-      <c r="U34" s="40"/>
-      <c r="V34" s="40"/>
-      <c r="W34" s="40"/>
-      <c r="X34" s="40"/>
-      <c r="Y34" s="40"/>
-      <c r="Z34" s="40"/>
-      <c r="AA34" s="40"/>
-      <c r="AB34" s="40"/>
-      <c r="AC34" s="40"/>
-      <c r="AD34" s="40"/>
-      <c r="AE34" s="40"/>
-      <c r="AF34" s="40"/>
-      <c r="AG34" s="40"/>
-      <c r="AH34" s="40"/>
-      <c r="AI34" s="40"/>
-      <c r="AJ34" s="40"/>
-      <c r="AK34" s="40"/>
-      <c r="AL34" s="40"/>
-      <c r="AM34" s="40"/>
-      <c r="AN34" s="40"/>
-      <c r="AO34" s="41"/>
+      <c r="C34" s="70"/>
+      <c r="D34" s="70"/>
+      <c r="E34" s="70"/>
+      <c r="F34" s="70"/>
+      <c r="G34" s="70"/>
+      <c r="H34" s="70"/>
+      <c r="I34" s="70"/>
+      <c r="J34" s="70"/>
+      <c r="K34" s="70"/>
+      <c r="L34" s="70"/>
+      <c r="M34" s="70"/>
+      <c r="N34" s="70"/>
+      <c r="O34" s="70"/>
+      <c r="P34" s="70"/>
+      <c r="Q34" s="70"/>
+      <c r="R34" s="70"/>
+      <c r="S34" s="70"/>
+      <c r="T34" s="70"/>
+      <c r="U34" s="70"/>
+      <c r="V34" s="70"/>
+      <c r="W34" s="70"/>
+      <c r="X34" s="70"/>
+      <c r="Y34" s="70"/>
+      <c r="Z34" s="70"/>
+      <c r="AA34" s="70"/>
+      <c r="AB34" s="70"/>
+      <c r="AC34" s="70"/>
+      <c r="AD34" s="70"/>
+      <c r="AE34" s="70"/>
+      <c r="AF34" s="70"/>
+      <c r="AG34" s="70"/>
+      <c r="AH34" s="70"/>
+      <c r="AI34" s="70"/>
+      <c r="AJ34" s="70"/>
+      <c r="AK34" s="70"/>
+      <c r="AL34" s="70"/>
+      <c r="AM34" s="70"/>
+      <c r="AN34" s="70"/>
+      <c r="AO34" s="71"/>
     </row>
     <row r="35" spans="1:41" ht="12.75">
       <c r="A35" s="6"/>
@@ -3123,13 +3131,13 @@
       <c r="AK35" s="38" t="s">
         <v>50</v>
       </c>
-      <c r="AL35" s="42">
+      <c r="AL35" s="72">
         <f>SUM(AL29:AN34)</f>
         <v>135000</v>
       </c>
-      <c r="AM35" s="42"/>
-      <c r="AN35" s="42"/>
-      <c r="AO35" s="43"/>
+      <c r="AM35" s="72"/>
+      <c r="AN35" s="72"/>
+      <c r="AO35" s="73"/>
     </row>
     <row r="36" spans="1:41" ht="12.75">
       <c r="A36" s="6"/>
@@ -3220,15 +3228,15 @@
     <row r="38" spans="1:41" ht="15">
       <c r="A38" s="6"/>
       <c r="B38" s="15"/>
-      <c r="C38" s="44" t="s">
+      <c r="C38" s="74" t="s">
         <v>65</v>
       </c>
-      <c r="D38" s="44"/>
-      <c r="E38" s="44"/>
-      <c r="F38" s="44"/>
-      <c r="G38" s="44"/>
-      <c r="H38" s="44"/>
-      <c r="I38" s="44"/>
+      <c r="D38" s="74"/>
+      <c r="E38" s="74"/>
+      <c r="F38" s="74"/>
+      <c r="G38" s="74"/>
+      <c r="H38" s="74"/>
+      <c r="I38" s="74"/>
       <c r="J38" s="23"/>
       <c r="K38" s="23"/>
       <c r="L38" s="23"/>
@@ -3265,175 +3273,175 @@
     <row r="39" spans="1:41" ht="12.75">
       <c r="A39" s="6"/>
       <c r="B39" s="15"/>
-      <c r="C39" s="45" t="s">
+      <c r="C39" s="75" t="s">
         <v>66</v>
       </c>
-      <c r="D39" s="45"/>
-      <c r="E39" s="45"/>
-      <c r="F39" s="45"/>
-      <c r="G39" s="45"/>
-      <c r="H39" s="45"/>
-      <c r="I39" s="45"/>
-      <c r="J39" s="45"/>
-      <c r="K39" s="45"/>
-      <c r="L39" s="45"/>
-      <c r="M39" s="45"/>
-      <c r="N39" s="45"/>
-      <c r="O39" s="45"/>
-      <c r="P39" s="45"/>
-      <c r="Q39" s="45"/>
-      <c r="R39" s="45"/>
-      <c r="S39" s="45"/>
-      <c r="T39" s="45"/>
-      <c r="U39" s="45"/>
-      <c r="V39" s="45"/>
-      <c r="W39" s="45"/>
-      <c r="X39" s="45"/>
-      <c r="Y39" s="45"/>
-      <c r="Z39" s="45"/>
-      <c r="AA39" s="45"/>
-      <c r="AB39" s="45"/>
-      <c r="AC39" s="45"/>
-      <c r="AD39" s="45"/>
-      <c r="AE39" s="45"/>
-      <c r="AF39" s="45"/>
-      <c r="AG39" s="45"/>
-      <c r="AH39" s="45"/>
-      <c r="AI39" s="45"/>
-      <c r="AJ39" s="45"/>
-      <c r="AK39" s="45"/>
-      <c r="AL39" s="45"/>
-      <c r="AM39" s="45"/>
-      <c r="AN39" s="45"/>
+      <c r="D39" s="75"/>
+      <c r="E39" s="75"/>
+      <c r="F39" s="75"/>
+      <c r="G39" s="75"/>
+      <c r="H39" s="75"/>
+      <c r="I39" s="75"/>
+      <c r="J39" s="75"/>
+      <c r="K39" s="75"/>
+      <c r="L39" s="75"/>
+      <c r="M39" s="75"/>
+      <c r="N39" s="75"/>
+      <c r="O39" s="75"/>
+      <c r="P39" s="75"/>
+      <c r="Q39" s="75"/>
+      <c r="R39" s="75"/>
+      <c r="S39" s="75"/>
+      <c r="T39" s="75"/>
+      <c r="U39" s="75"/>
+      <c r="V39" s="75"/>
+      <c r="W39" s="75"/>
+      <c r="X39" s="75"/>
+      <c r="Y39" s="75"/>
+      <c r="Z39" s="75"/>
+      <c r="AA39" s="75"/>
+      <c r="AB39" s="75"/>
+      <c r="AC39" s="75"/>
+      <c r="AD39" s="75"/>
+      <c r="AE39" s="75"/>
+      <c r="AF39" s="75"/>
+      <c r="AG39" s="75"/>
+      <c r="AH39" s="75"/>
+      <c r="AI39" s="75"/>
+      <c r="AJ39" s="75"/>
+      <c r="AK39" s="75"/>
+      <c r="AL39" s="75"/>
+      <c r="AM39" s="75"/>
+      <c r="AN39" s="75"/>
       <c r="AO39" s="18"/>
     </row>
     <row r="40" spans="1:41" ht="12.75">
       <c r="A40" s="6"/>
       <c r="B40" s="15"/>
-      <c r="C40" s="45"/>
-      <c r="D40" s="45"/>
-      <c r="E40" s="45"/>
-      <c r="F40" s="45"/>
-      <c r="G40" s="45"/>
-      <c r="H40" s="45"/>
-      <c r="I40" s="45"/>
-      <c r="J40" s="45"/>
-      <c r="K40" s="45"/>
-      <c r="L40" s="45"/>
-      <c r="M40" s="45"/>
-      <c r="N40" s="45"/>
-      <c r="O40" s="45"/>
-      <c r="P40" s="45"/>
-      <c r="Q40" s="45"/>
-      <c r="R40" s="45"/>
-      <c r="S40" s="45"/>
-      <c r="T40" s="45"/>
-      <c r="U40" s="45"/>
-      <c r="V40" s="45"/>
-      <c r="W40" s="45"/>
-      <c r="X40" s="45"/>
-      <c r="Y40" s="45"/>
-      <c r="Z40" s="45"/>
-      <c r="AA40" s="45"/>
-      <c r="AB40" s="45"/>
-      <c r="AC40" s="45"/>
-      <c r="AD40" s="45"/>
-      <c r="AE40" s="45"/>
-      <c r="AF40" s="45"/>
-      <c r="AG40" s="45"/>
-      <c r="AH40" s="45"/>
-      <c r="AI40" s="45"/>
-      <c r="AJ40" s="45"/>
-      <c r="AK40" s="45"/>
-      <c r="AL40" s="45"/>
-      <c r="AM40" s="45"/>
-      <c r="AN40" s="45"/>
+      <c r="C40" s="75"/>
+      <c r="D40" s="75"/>
+      <c r="E40" s="75"/>
+      <c r="F40" s="75"/>
+      <c r="G40" s="75"/>
+      <c r="H40" s="75"/>
+      <c r="I40" s="75"/>
+      <c r="J40" s="75"/>
+      <c r="K40" s="75"/>
+      <c r="L40" s="75"/>
+      <c r="M40" s="75"/>
+      <c r="N40" s="75"/>
+      <c r="O40" s="75"/>
+      <c r="P40" s="75"/>
+      <c r="Q40" s="75"/>
+      <c r="R40" s="75"/>
+      <c r="S40" s="75"/>
+      <c r="T40" s="75"/>
+      <c r="U40" s="75"/>
+      <c r="V40" s="75"/>
+      <c r="W40" s="75"/>
+      <c r="X40" s="75"/>
+      <c r="Y40" s="75"/>
+      <c r="Z40" s="75"/>
+      <c r="AA40" s="75"/>
+      <c r="AB40" s="75"/>
+      <c r="AC40" s="75"/>
+      <c r="AD40" s="75"/>
+      <c r="AE40" s="75"/>
+      <c r="AF40" s="75"/>
+      <c r="AG40" s="75"/>
+      <c r="AH40" s="75"/>
+      <c r="AI40" s="75"/>
+      <c r="AJ40" s="75"/>
+      <c r="AK40" s="75"/>
+      <c r="AL40" s="75"/>
+      <c r="AM40" s="75"/>
+      <c r="AN40" s="75"/>
       <c r="AO40" s="18"/>
     </row>
     <row r="41" spans="1:41" ht="12.75">
       <c r="A41" s="6"/>
       <c r="B41" s="15"/>
-      <c r="C41" s="45"/>
-      <c r="D41" s="45"/>
-      <c r="E41" s="45"/>
-      <c r="F41" s="45"/>
-      <c r="G41" s="45"/>
-      <c r="H41" s="45"/>
-      <c r="I41" s="45"/>
-      <c r="J41" s="45"/>
-      <c r="K41" s="45"/>
-      <c r="L41" s="45"/>
-      <c r="M41" s="45"/>
-      <c r="N41" s="45"/>
-      <c r="O41" s="45"/>
-      <c r="P41" s="45"/>
-      <c r="Q41" s="45"/>
-      <c r="R41" s="45"/>
-      <c r="S41" s="45"/>
-      <c r="T41" s="45"/>
-      <c r="U41" s="45"/>
-      <c r="V41" s="45"/>
-      <c r="W41" s="45"/>
-      <c r="X41" s="45"/>
-      <c r="Y41" s="45"/>
-      <c r="Z41" s="45"/>
-      <c r="AA41" s="45"/>
-      <c r="AB41" s="45"/>
-      <c r="AC41" s="45"/>
-      <c r="AD41" s="45"/>
-      <c r="AE41" s="45"/>
-      <c r="AF41" s="45"/>
-      <c r="AG41" s="45"/>
-      <c r="AH41" s="45"/>
-      <c r="AI41" s="45"/>
-      <c r="AJ41" s="45"/>
-      <c r="AK41" s="45"/>
-      <c r="AL41" s="45"/>
-      <c r="AM41" s="45"/>
-      <c r="AN41" s="45"/>
+      <c r="C41" s="75"/>
+      <c r="D41" s="75"/>
+      <c r="E41" s="75"/>
+      <c r="F41" s="75"/>
+      <c r="G41" s="75"/>
+      <c r="H41" s="75"/>
+      <c r="I41" s="75"/>
+      <c r="J41" s="75"/>
+      <c r="K41" s="75"/>
+      <c r="L41" s="75"/>
+      <c r="M41" s="75"/>
+      <c r="N41" s="75"/>
+      <c r="O41" s="75"/>
+      <c r="P41" s="75"/>
+      <c r="Q41" s="75"/>
+      <c r="R41" s="75"/>
+      <c r="S41" s="75"/>
+      <c r="T41" s="75"/>
+      <c r="U41" s="75"/>
+      <c r="V41" s="75"/>
+      <c r="W41" s="75"/>
+      <c r="X41" s="75"/>
+      <c r="Y41" s="75"/>
+      <c r="Z41" s="75"/>
+      <c r="AA41" s="75"/>
+      <c r="AB41" s="75"/>
+      <c r="AC41" s="75"/>
+      <c r="AD41" s="75"/>
+      <c r="AE41" s="75"/>
+      <c r="AF41" s="75"/>
+      <c r="AG41" s="75"/>
+      <c r="AH41" s="75"/>
+      <c r="AI41" s="75"/>
+      <c r="AJ41" s="75"/>
+      <c r="AK41" s="75"/>
+      <c r="AL41" s="75"/>
+      <c r="AM41" s="75"/>
+      <c r="AN41" s="75"/>
       <c r="AO41" s="18"/>
     </row>
     <row r="42" spans="1:41" ht="12.75">
       <c r="A42" s="6"/>
       <c r="B42" s="15"/>
-      <c r="C42" s="45"/>
-      <c r="D42" s="45"/>
-      <c r="E42" s="45"/>
-      <c r="F42" s="45"/>
-      <c r="G42" s="45"/>
-      <c r="H42" s="45"/>
-      <c r="I42" s="45"/>
-      <c r="J42" s="45"/>
-      <c r="K42" s="45"/>
-      <c r="L42" s="45"/>
-      <c r="M42" s="45"/>
-      <c r="N42" s="45"/>
-      <c r="O42" s="45"/>
-      <c r="P42" s="45"/>
-      <c r="Q42" s="45"/>
-      <c r="R42" s="45"/>
-      <c r="S42" s="45"/>
-      <c r="T42" s="45"/>
-      <c r="U42" s="45"/>
-      <c r="V42" s="45"/>
-      <c r="W42" s="45"/>
-      <c r="X42" s="45"/>
-      <c r="Y42" s="45"/>
-      <c r="Z42" s="45"/>
-      <c r="AA42" s="45"/>
-      <c r="AB42" s="45"/>
-      <c r="AC42" s="45"/>
-      <c r="AD42" s="45"/>
-      <c r="AE42" s="45"/>
-      <c r="AF42" s="45"/>
-      <c r="AG42" s="45"/>
-      <c r="AH42" s="45"/>
-      <c r="AI42" s="45"/>
-      <c r="AJ42" s="45"/>
-      <c r="AK42" s="45"/>
-      <c r="AL42" s="45"/>
-      <c r="AM42" s="45"/>
-      <c r="AN42" s="45"/>
+      <c r="C42" s="75"/>
+      <c r="D42" s="75"/>
+      <c r="E42" s="75"/>
+      <c r="F42" s="75"/>
+      <c r="G42" s="75"/>
+      <c r="H42" s="75"/>
+      <c r="I42" s="75"/>
+      <c r="J42" s="75"/>
+      <c r="K42" s="75"/>
+      <c r="L42" s="75"/>
+      <c r="M42" s="75"/>
+      <c r="N42" s="75"/>
+      <c r="O42" s="75"/>
+      <c r="P42" s="75"/>
+      <c r="Q42" s="75"/>
+      <c r="R42" s="75"/>
+      <c r="S42" s="75"/>
+      <c r="T42" s="75"/>
+      <c r="U42" s="75"/>
+      <c r="V42" s="75"/>
+      <c r="W42" s="75"/>
+      <c r="X42" s="75"/>
+      <c r="Y42" s="75"/>
+      <c r="Z42" s="75"/>
+      <c r="AA42" s="75"/>
+      <c r="AB42" s="75"/>
+      <c r="AC42" s="75"/>
+      <c r="AD42" s="75"/>
+      <c r="AE42" s="75"/>
+      <c r="AF42" s="75"/>
+      <c r="AG42" s="75"/>
+      <c r="AH42" s="75"/>
+      <c r="AI42" s="75"/>
+      <c r="AJ42" s="75"/>
+      <c r="AK42" s="75"/>
+      <c r="AL42" s="75"/>
+      <c r="AM42" s="75"/>
+      <c r="AN42" s="75"/>
       <c r="AO42" s="18"/>
     </row>
     <row r="43" spans="1:41" ht="12.75">
@@ -3524,67 +3532,92 @@
     </row>
     <row r="45" spans="1:41" ht="12.75">
       <c r="A45" s="6"/>
-      <c r="B45" s="46" t="s">
+      <c r="B45" s="76" t="s">
         <v>67</v>
       </c>
-      <c r="C45" s="46"/>
-      <c r="D45" s="46"/>
-      <c r="E45" s="46"/>
-      <c r="F45" s="46"/>
-      <c r="G45" s="46"/>
-      <c r="H45" s="46"/>
-      <c r="I45" s="46"/>
-      <c r="J45" s="46"/>
-      <c r="K45" s="46"/>
-      <c r="L45" s="46"/>
-      <c r="M45" s="46"/>
-      <c r="N45" s="46"/>
-      <c r="O45" s="46"/>
-      <c r="P45" s="46"/>
-      <c r="Q45" s="46"/>
-      <c r="R45" s="46"/>
-      <c r="S45" s="46"/>
-      <c r="T45" s="46"/>
-      <c r="U45" s="46"/>
-      <c r="V45" s="46"/>
-      <c r="W45" s="46"/>
-      <c r="X45" s="46"/>
-      <c r="Y45" s="46"/>
-      <c r="Z45" s="46"/>
-      <c r="AA45" s="46"/>
-      <c r="AB45" s="46"/>
-      <c r="AC45" s="46"/>
-      <c r="AD45" s="46"/>
-      <c r="AE45" s="46"/>
-      <c r="AF45" s="46"/>
-      <c r="AG45" s="46"/>
-      <c r="AH45" s="46"/>
-      <c r="AI45" s="46"/>
-      <c r="AJ45" s="46"/>
-      <c r="AK45" s="46"/>
-      <c r="AL45" s="46"/>
-      <c r="AM45" s="46"/>
-      <c r="AN45" s="46"/>
-      <c r="AO45" s="46"/>
+      <c r="C45" s="76"/>
+      <c r="D45" s="76"/>
+      <c r="E45" s="76"/>
+      <c r="F45" s="76"/>
+      <c r="G45" s="76"/>
+      <c r="H45" s="76"/>
+      <c r="I45" s="76"/>
+      <c r="J45" s="76"/>
+      <c r="K45" s="76"/>
+      <c r="L45" s="76"/>
+      <c r="M45" s="76"/>
+      <c r="N45" s="76"/>
+      <c r="O45" s="76"/>
+      <c r="P45" s="76"/>
+      <c r="Q45" s="76"/>
+      <c r="R45" s="76"/>
+      <c r="S45" s="76"/>
+      <c r="T45" s="76"/>
+      <c r="U45" s="76"/>
+      <c r="V45" s="76"/>
+      <c r="W45" s="76"/>
+      <c r="X45" s="76"/>
+      <c r="Y45" s="76"/>
+      <c r="Z45" s="76"/>
+      <c r="AA45" s="76"/>
+      <c r="AB45" s="76"/>
+      <c r="AC45" s="76"/>
+      <c r="AD45" s="76"/>
+      <c r="AE45" s="76"/>
+      <c r="AF45" s="76"/>
+      <c r="AG45" s="76"/>
+      <c r="AH45" s="76"/>
+      <c r="AI45" s="76"/>
+      <c r="AJ45" s="76"/>
+      <c r="AK45" s="76"/>
+      <c r="AL45" s="76"/>
+      <c r="AM45" s="76"/>
+      <c r="AN45" s="76"/>
+      <c r="AO45" s="76"/>
     </row>
   </sheetData>
   <mergeCells count="72">
-    <mergeCell ref="W7:Y7"/>
-    <mergeCell ref="G1:AK1"/>
-    <mergeCell ref="G2:AL2"/>
-    <mergeCell ref="G3:AL3"/>
-    <mergeCell ref="G4:AL4"/>
-    <mergeCell ref="AG5:AO5"/>
-    <mergeCell ref="C18:T21"/>
-    <mergeCell ref="AC18:AK18"/>
-    <mergeCell ref="AC19:AJ19"/>
-    <mergeCell ref="AC20:AK20"/>
-    <mergeCell ref="AC21:AH21"/>
-    <mergeCell ref="C8:T13"/>
-    <mergeCell ref="W8:AN13"/>
-    <mergeCell ref="AC16:AK16"/>
-    <mergeCell ref="C17:E17"/>
-    <mergeCell ref="AC17:AK17"/>
+    <mergeCell ref="B34:AO34"/>
+    <mergeCell ref="AL35:AO35"/>
+    <mergeCell ref="C38:I38"/>
+    <mergeCell ref="C39:AN42"/>
+    <mergeCell ref="B45:AO45"/>
+    <mergeCell ref="AL33:AO33"/>
+    <mergeCell ref="C32:F32"/>
+    <mergeCell ref="H32:J32"/>
+    <mergeCell ref="R32:AD32"/>
+    <mergeCell ref="AE32:AF32"/>
+    <mergeCell ref="AH32:AJ32"/>
+    <mergeCell ref="AL32:AO32"/>
+    <mergeCell ref="C33:F33"/>
+    <mergeCell ref="H33:J33"/>
+    <mergeCell ref="R33:AD33"/>
+    <mergeCell ref="AE33:AF33"/>
+    <mergeCell ref="AH33:AJ33"/>
+    <mergeCell ref="L32:P32"/>
+    <mergeCell ref="L33:P33"/>
+    <mergeCell ref="AL31:AO31"/>
+    <mergeCell ref="C30:F30"/>
+    <mergeCell ref="H30:J30"/>
+    <mergeCell ref="R30:AD30"/>
+    <mergeCell ref="AE30:AF30"/>
+    <mergeCell ref="AH30:AJ30"/>
+    <mergeCell ref="AL30:AO30"/>
+    <mergeCell ref="C31:F31"/>
+    <mergeCell ref="H31:J31"/>
+    <mergeCell ref="R31:AD31"/>
+    <mergeCell ref="AE31:AF31"/>
+    <mergeCell ref="AH31:AJ31"/>
+    <mergeCell ref="L30:P30"/>
+    <mergeCell ref="L31:P31"/>
+    <mergeCell ref="B28:AO28"/>
+    <mergeCell ref="C29:F29"/>
+    <mergeCell ref="H29:J29"/>
+    <mergeCell ref="R29:AD29"/>
+    <mergeCell ref="AE29:AF29"/>
+    <mergeCell ref="AH29:AJ29"/>
+    <mergeCell ref="AL29:AO29"/>
+    <mergeCell ref="L29:P29"/>
     <mergeCell ref="AC22:AH22"/>
     <mergeCell ref="AL24:AN24"/>
     <mergeCell ref="C25:F26"/>
@@ -3600,47 +3633,22 @@
     <mergeCell ref="L22:N22"/>
     <mergeCell ref="O22:Q22"/>
     <mergeCell ref="R22:T22"/>
-    <mergeCell ref="B28:AO28"/>
-    <mergeCell ref="C29:F29"/>
-    <mergeCell ref="H29:J29"/>
-    <mergeCell ref="R29:AD29"/>
-    <mergeCell ref="AE29:AF29"/>
-    <mergeCell ref="AH29:AJ29"/>
-    <mergeCell ref="AL29:AO29"/>
-    <mergeCell ref="L29:P29"/>
-    <mergeCell ref="AL31:AO31"/>
-    <mergeCell ref="C30:F30"/>
-    <mergeCell ref="H30:J30"/>
-    <mergeCell ref="R30:AD30"/>
-    <mergeCell ref="AE30:AF30"/>
-    <mergeCell ref="AH30:AJ30"/>
-    <mergeCell ref="AL30:AO30"/>
-    <mergeCell ref="C31:F31"/>
-    <mergeCell ref="H31:J31"/>
-    <mergeCell ref="R31:AD31"/>
-    <mergeCell ref="AE31:AF31"/>
-    <mergeCell ref="AH31:AJ31"/>
-    <mergeCell ref="L30:P30"/>
-    <mergeCell ref="L31:P31"/>
-    <mergeCell ref="AL33:AO33"/>
-    <mergeCell ref="C32:F32"/>
-    <mergeCell ref="H32:J32"/>
-    <mergeCell ref="R32:AD32"/>
-    <mergeCell ref="AE32:AF32"/>
-    <mergeCell ref="AH32:AJ32"/>
-    <mergeCell ref="AL32:AO32"/>
-    <mergeCell ref="C33:F33"/>
-    <mergeCell ref="H33:J33"/>
-    <mergeCell ref="R33:AD33"/>
-    <mergeCell ref="AE33:AF33"/>
-    <mergeCell ref="AH33:AJ33"/>
-    <mergeCell ref="L32:P32"/>
-    <mergeCell ref="L33:P33"/>
-    <mergeCell ref="B34:AO34"/>
-    <mergeCell ref="AL35:AO35"/>
-    <mergeCell ref="C38:I38"/>
-    <mergeCell ref="C39:AN42"/>
-    <mergeCell ref="B45:AO45"/>
+    <mergeCell ref="C8:T13"/>
+    <mergeCell ref="W8:AN13"/>
+    <mergeCell ref="AC16:AK16"/>
+    <mergeCell ref="C17:E17"/>
+    <mergeCell ref="AC17:AK17"/>
+    <mergeCell ref="C18:T21"/>
+    <mergeCell ref="AC18:AK18"/>
+    <mergeCell ref="AC19:AJ19"/>
+    <mergeCell ref="AC20:AK20"/>
+    <mergeCell ref="AC21:AH21"/>
+    <mergeCell ref="W7:Y7"/>
+    <mergeCell ref="G1:AK1"/>
+    <mergeCell ref="G2:AL2"/>
+    <mergeCell ref="G3:AL3"/>
+    <mergeCell ref="G4:AL4"/>
+    <mergeCell ref="AG5:AO5"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <dataValidations count="1">

</xml_diff>